<commit_message>
eboighar test case added
</commit_message>
<xml_diff>
--- a/B.eboighor_signup.xlsx
+++ b/B.eboighor_signup.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="158">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -333,9 +333,6 @@
     <t>TC-13</t>
   </si>
   <si>
-    <t>Mamunbooks</t>
-  </si>
-  <si>
     <t>SignUp</t>
   </si>
   <si>
@@ -445,12 +442,175 @@
 4.Name field with digit.
 5.Click signup button(ER-1, ER-2).</t>
   </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>1.Name: p</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Name field input single character.
+5.Click signup button(ER-1, ER-2).</t>
+  </si>
+  <si>
+    <t>1.User should get a warning "invalid name."
+2.user should not able to use single character.</t>
+  </si>
+  <si>
+    <t>1.User not get warning message.
+2.User able to use single character.</t>
+  </si>
+  <si>
+    <t>Validate Name field into  single character value to see allowed or not</t>
+  </si>
+  <si>
+    <t>Validate Name field into character and special character to see allowed or not</t>
+  </si>
+  <si>
+    <t>1.Name: pa@roy</t>
+  </si>
+  <si>
+    <t>1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Name field input character and special character.
+5.Click signup button(ER-1).</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Validate Mobile field with valid mobile number.</t>
+  </si>
+  <si>
+    <t>1.Mobile: 01737629976</t>
+  </si>
+  <si>
+    <t>1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Input Valid mobile number.
+5.Click signup button(ER-1).</t>
+  </si>
+  <si>
+    <t>1.User able to use valid mobile number.</t>
+  </si>
+  <si>
+    <t>1.user able to use special character.</t>
+  </si>
+  <si>
+    <t>Validate Mobile field with number and character and special character to see allowed or not.</t>
+  </si>
+  <si>
+    <t>1.Mobile: 017a7629976.
+2.Mobile:
+017@729976.</t>
+  </si>
+  <si>
+    <t>1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Input mobile number mixed line character,number.
+5.Click signup button(ER-1).</t>
+  </si>
+  <si>
+    <t>1.User should be able to use valid mobile number.</t>
+  </si>
+  <si>
+    <t>1.User should be able to use special character.</t>
+  </si>
+  <si>
+    <t>1.The user should get warning " Online number are allowed"
+2.The user should not be able to use characters and special characters on a mobile field.</t>
+  </si>
+  <si>
+    <t>1.User not able to use character and special character.</t>
+  </si>
+  <si>
+    <t>Validate Mobile Number to see if it is unique. </t>
+  </si>
+  <si>
+    <t>1.Mobile:01737629976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The user should get warning " mobile number already used"
+2.The user should not be able to use one mobile number twice. </t>
+  </si>
+  <si>
+    <t>1.User not able to use one mobile number twice.</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>1.Email: pari@gmai.com</t>
+  </si>
+  <si>
+    <t>1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Email field with valid email address.
+5.Click signup button(ER-1).</t>
+  </si>
+  <si>
+    <t>1.User should able to use valid email address.</t>
+  </si>
+  <si>
+    <t>1.User able to use valid email address.</t>
+  </si>
+  <si>
+    <t>Validate Email field into valid email address to see allowed or not.</t>
+  </si>
+  <si>
+    <t>Validate Email field into invalid email address to see allowed or not</t>
+  </si>
+  <si>
+    <t>1.Email:
+@gmai.com
+2.Email:
+pa@gmail
+3.Email:
+pa@gmail-com</t>
+  </si>
+  <si>
+    <t>1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Email field with invalid email address.
+5.Click signup button(ER-1.ER-2).</t>
+  </si>
+  <si>
+    <t>1.open an application( https://eboighar.com/ ) in any browser
+2. Click on Log in button.
+3.Click on Sign up button.
+4.Input used mobile number.
+5.Click signup button(ER-1,ER-2).</t>
+  </si>
+  <si>
+    <t>.1.User should ge warning " invalid email address"
+2.User should not be able to use invalid email address.</t>
+  </si>
+  <si>
+    <t>1.User not able to use invalid mobile number.</t>
+  </si>
+  <si>
+    <t>TC-004</t>
+  </si>
+  <si>
+    <t>Eboighar</t>
+  </si>
+  <si>
+    <t>Click here</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="39">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -674,6 +834,16 @@
     <font>
       <sz val="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1423,7 +1593,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1981,6 +2151,12 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2047,12 +2223,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2098,7 +2268,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2107,22 +2280,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2130,12 +2300,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2218,13 +2382,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2232,9 +2390,6 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2250,12 +2405,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2310,11 +2459,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="16" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2331,8 +2483,14 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2590,10 +2748,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2887,9 +3045,8 @@
   </sheetPr>
   <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:A32"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2911,16 +3068,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="164" customFormat="1" ht="15" customHeight="1">
-      <c r="F1" s="326" t="s">
+      <c r="F1" s="320" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="327"/>
+      <c r="G1" s="321"/>
     </row>
     <row r="2" spans="1:29" s="164" customFormat="1" ht="15" customHeight="1">
-      <c r="D2" s="324" t="s">
+      <c r="D2" s="318" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="325"/>
+      <c r="E2" s="319"/>
       <c r="F2" s="198"/>
     </row>
     <row r="3" spans="1:29" s="164" customFormat="1" ht="15" customHeight="1">
@@ -2928,7 +3085,7 @@
         <v>69</v>
       </c>
       <c r="E3" s="170" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="F3" s="198"/>
     </row>
@@ -2948,10 +3105,10 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="276" t="s">
+      <c r="L4" s="274" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="277"/>
+      <c r="M4" s="275"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
@@ -2990,7 +3147,7 @@
       </c>
       <c r="M5" s="6">
         <f>COUNTIF(L12:L471, "Passed")</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -3028,7 +3185,7 @@
       </c>
       <c r="M6" s="6">
         <f>COUNTIF(L12:L471, "Failed")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3131,7 +3288,7 @@
         <v>83</v>
       </c>
       <c r="E9" s="192" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="199"/>
       <c r="G9" s="1"/>
@@ -3174,7 +3331,7 @@
       </c>
       <c r="M10" s="12">
         <f>SUM(M5:M8)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -3216,10 +3373,10 @@
         <v>12</v>
       </c>
       <c r="H11" s="172" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I11" s="172" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J11" s="172" t="s">
         <v>13</v>
@@ -3251,36 +3408,36 @@
       <c r="AC11" s="173"/>
     </row>
     <row r="12" spans="1:29" ht="30" customHeight="1">
-      <c r="A12" s="299" t="s">
+      <c r="A12" s="294" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="318" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="320" t="s">
+      <c r="B12" s="311" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="313" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="316" t="s">
+      <c r="D12" s="309" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="248" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="303" t="s">
+      <c r="F12" s="278" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="280" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="303" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="303" t="s">
+      <c r="G12" s="248" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="248" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="303" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="310" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="304"/>
-      <c r="K12" s="307"/>
-      <c r="L12" s="209" t="s">
+      <c r="J12" s="297"/>
+      <c r="K12" s="300"/>
+      <c r="L12" s="211" t="s">
         <v>77</v>
       </c>
       <c r="M12" s="168"/>
@@ -3302,18 +3459,18 @@
       <c r="AC12" s="4"/>
     </row>
     <row r="13" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A13" s="300"/>
-      <c r="B13" s="319"/>
-      <c r="C13" s="321"/>
-      <c r="D13" s="317"/>
-      <c r="E13" s="313"/>
-      <c r="F13" s="281"/>
+      <c r="A13" s="295"/>
+      <c r="B13" s="312"/>
+      <c r="C13" s="314"/>
+      <c r="D13" s="310"/>
+      <c r="E13" s="306"/>
+      <c r="F13" s="279"/>
       <c r="G13" s="238"/>
-      <c r="H13" s="313"/>
-      <c r="I13" s="311"/>
-      <c r="J13" s="305"/>
-      <c r="K13" s="308"/>
-      <c r="L13" s="210"/>
+      <c r="H13" s="306"/>
+      <c r="I13" s="304"/>
+      <c r="J13" s="298"/>
+      <c r="K13" s="301"/>
+      <c r="L13" s="212"/>
       <c r="M13" s="167"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -3333,18 +3490,18 @@
       <c r="AC13" s="4"/>
     </row>
     <row r="14" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A14" s="300"/>
-      <c r="B14" s="319"/>
-      <c r="C14" s="321"/>
-      <c r="D14" s="317"/>
-      <c r="E14" s="313"/>
-      <c r="F14" s="281"/>
+      <c r="A14" s="295"/>
+      <c r="B14" s="312"/>
+      <c r="C14" s="314"/>
+      <c r="D14" s="310"/>
+      <c r="E14" s="306"/>
+      <c r="F14" s="279"/>
       <c r="G14" s="238"/>
-      <c r="H14" s="313"/>
-      <c r="I14" s="311"/>
-      <c r="J14" s="305"/>
-      <c r="K14" s="308"/>
-      <c r="L14" s="210"/>
+      <c r="H14" s="306"/>
+      <c r="I14" s="304"/>
+      <c r="J14" s="298"/>
+      <c r="K14" s="301"/>
+      <c r="L14" s="212"/>
       <c r="M14" s="162"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -3364,18 +3521,18 @@
       <c r="AC14" s="4"/>
     </row>
     <row r="15" spans="1:29" ht="25.5" customHeight="1">
-      <c r="A15" s="300"/>
-      <c r="B15" s="319"/>
-      <c r="C15" s="321"/>
-      <c r="D15" s="317"/>
-      <c r="E15" s="313"/>
-      <c r="F15" s="281"/>
+      <c r="A15" s="295"/>
+      <c r="B15" s="312"/>
+      <c r="C15" s="314"/>
+      <c r="D15" s="310"/>
+      <c r="E15" s="306"/>
+      <c r="F15" s="279"/>
       <c r="G15" s="238"/>
-      <c r="H15" s="313"/>
-      <c r="I15" s="311"/>
-      <c r="J15" s="305"/>
-      <c r="K15" s="308"/>
-      <c r="L15" s="210"/>
+      <c r="H15" s="306"/>
+      <c r="I15" s="304"/>
+      <c r="J15" s="298"/>
+      <c r="K15" s="301"/>
+      <c r="L15" s="212"/>
       <c r="M15" s="162"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -3395,18 +3552,18 @@
       <c r="AC15" s="4"/>
     </row>
     <row r="16" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A16" s="300"/>
-      <c r="B16" s="319"/>
-      <c r="C16" s="321"/>
-      <c r="D16" s="317"/>
-      <c r="E16" s="313"/>
-      <c r="F16" s="281"/>
+      <c r="A16" s="295"/>
+      <c r="B16" s="312"/>
+      <c r="C16" s="314"/>
+      <c r="D16" s="310"/>
+      <c r="E16" s="306"/>
+      <c r="F16" s="279"/>
       <c r="G16" s="238"/>
-      <c r="H16" s="313"/>
-      <c r="I16" s="311"/>
-      <c r="J16" s="305"/>
-      <c r="K16" s="308"/>
-      <c r="L16" s="210"/>
+      <c r="H16" s="306"/>
+      <c r="I16" s="304"/>
+      <c r="J16" s="298"/>
+      <c r="K16" s="301"/>
+      <c r="L16" s="212"/>
       <c r="M16" s="162"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -3426,18 +3583,18 @@
       <c r="AC16" s="4"/>
     </row>
     <row r="17" spans="1:29" s="161" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="300"/>
-      <c r="B17" s="319"/>
-      <c r="C17" s="321"/>
-      <c r="D17" s="317"/>
-      <c r="E17" s="313"/>
-      <c r="F17" s="281"/>
+      <c r="A17" s="295"/>
+      <c r="B17" s="312"/>
+      <c r="C17" s="314"/>
+      <c r="D17" s="310"/>
+      <c r="E17" s="306"/>
+      <c r="F17" s="279"/>
       <c r="G17" s="238"/>
-      <c r="H17" s="313"/>
-      <c r="I17" s="311"/>
-      <c r="J17" s="305"/>
-      <c r="K17" s="308"/>
-      <c r="L17" s="210"/>
+      <c r="H17" s="306"/>
+      <c r="I17" s="304"/>
+      <c r="J17" s="298"/>
+      <c r="K17" s="301"/>
+      <c r="L17" s="212"/>
       <c r="M17" s="162"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -3457,18 +3614,18 @@
       <c r="AC17" s="4"/>
     </row>
     <row r="18" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A18" s="301"/>
-      <c r="B18" s="319"/>
-      <c r="C18" s="321"/>
-      <c r="D18" s="317"/>
-      <c r="E18" s="314"/>
-      <c r="F18" s="282"/>
+      <c r="A18" s="296"/>
+      <c r="B18" s="312"/>
+      <c r="C18" s="314"/>
+      <c r="D18" s="310"/>
+      <c r="E18" s="307"/>
+      <c r="F18" s="280"/>
       <c r="G18" s="247"/>
-      <c r="H18" s="314"/>
-      <c r="I18" s="312"/>
-      <c r="J18" s="306"/>
-      <c r="K18" s="309"/>
-      <c r="L18" s="211"/>
+      <c r="H18" s="307"/>
+      <c r="I18" s="305"/>
+      <c r="J18" s="299"/>
+      <c r="K18" s="302"/>
+      <c r="L18" s="213"/>
       <c r="M18" s="163"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -3492,26 +3649,26 @@
         <v>78</v>
       </c>
       <c r="B19" s="206" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="107"/>
+      <c r="D19" s="322" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="107"/>
-      <c r="D19" s="328" t="s">
+      <c r="E19" s="175" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="175" t="s">
+      <c r="F19" s="207" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="207" t="s">
-        <v>102</v>
-      </c>
       <c r="G19" s="208" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="175" t="s">
+      <c r="I19" s="175" t="s">
         <v>105</v>
-      </c>
-      <c r="I19" s="175" t="s">
-        <v>106</v>
       </c>
       <c r="J19" s="166"/>
       <c r="K19" s="165"/>
@@ -3537,30 +3694,30 @@
       <c r="AC19" s="4"/>
     </row>
     <row r="20" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A20" s="209" t="s">
+      <c r="A20" s="211" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="328"/>
-      <c r="C20" s="210"/>
-      <c r="D20" s="328"/>
+      <c r="B20" s="322"/>
+      <c r="C20" s="212"/>
+      <c r="D20" s="322"/>
       <c r="E20" s="238" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="254" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="259" t="s">
+      <c r="G20" s="286" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="238" t="s">
         <v>108</v>
       </c>
-      <c r="G20" s="288" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20" s="238" t="s">
+      <c r="I20" s="238" t="s">
         <v>109</v>
       </c>
-      <c r="I20" s="238" t="s">
-        <v>110</v>
-      </c>
-      <c r="J20" s="283"/>
+      <c r="J20" s="281"/>
       <c r="K20" s="238"/>
-      <c r="L20" s="210" t="s">
+      <c r="L20" s="212" t="s">
         <v>77</v>
       </c>
       <c r="M20" s="27"/>
@@ -3582,18 +3739,18 @@
       <c r="AC20" s="4"/>
     </row>
     <row r="21" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A21" s="210"/>
-      <c r="B21" s="328"/>
-      <c r="C21" s="210"/>
-      <c r="D21" s="328"/>
+      <c r="A21" s="212"/>
+      <c r="B21" s="322"/>
+      <c r="C21" s="212"/>
+      <c r="D21" s="322"/>
       <c r="E21" s="238"/>
-      <c r="F21" s="259"/>
-      <c r="G21" s="289"/>
+      <c r="F21" s="254"/>
+      <c r="G21" s="287"/>
       <c r="H21" s="238"/>
       <c r="I21" s="238"/>
-      <c r="J21" s="283"/>
+      <c r="J21" s="281"/>
       <c r="K21" s="238"/>
-      <c r="L21" s="210"/>
+      <c r="L21" s="212"/>
       <c r="M21" s="28"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -3613,18 +3770,18 @@
       <c r="AC21" s="4"/>
     </row>
     <row r="22" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A22" s="210"/>
-      <c r="B22" s="328"/>
-      <c r="C22" s="210"/>
-      <c r="D22" s="328"/>
+      <c r="A22" s="212"/>
+      <c r="B22" s="322"/>
+      <c r="C22" s="212"/>
+      <c r="D22" s="322"/>
       <c r="E22" s="238"/>
-      <c r="F22" s="259"/>
-      <c r="G22" s="289"/>
+      <c r="F22" s="254"/>
+      <c r="G22" s="287"/>
       <c r="H22" s="238"/>
       <c r="I22" s="238"/>
-      <c r="J22" s="283"/>
+      <c r="J22" s="281"/>
       <c r="K22" s="238"/>
-      <c r="L22" s="210"/>
+      <c r="L22" s="212"/>
       <c r="M22" s="28"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -3644,18 +3801,18 @@
       <c r="AC22" s="4"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A23" s="210"/>
-      <c r="B23" s="328"/>
-      <c r="C23" s="210"/>
-      <c r="D23" s="328"/>
+      <c r="A23" s="212"/>
+      <c r="B23" s="322"/>
+      <c r="C23" s="212"/>
+      <c r="D23" s="322"/>
       <c r="E23" s="238"/>
-      <c r="F23" s="259"/>
-      <c r="G23" s="289"/>
+      <c r="F23" s="254"/>
+      <c r="G23" s="287"/>
       <c r="H23" s="238"/>
       <c r="I23" s="238"/>
-      <c r="J23" s="283"/>
+      <c r="J23" s="281"/>
       <c r="K23" s="238"/>
-      <c r="L23" s="210"/>
+      <c r="L23" s="212"/>
       <c r="M23" s="30"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -3675,18 +3832,18 @@
       <c r="AC23" s="4"/>
     </row>
     <row r="24" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A24" s="210"/>
-      <c r="B24" s="328"/>
-      <c r="C24" s="210"/>
-      <c r="D24" s="328"/>
+      <c r="A24" s="212"/>
+      <c r="B24" s="322"/>
+      <c r="C24" s="212"/>
+      <c r="D24" s="322"/>
       <c r="E24" s="238"/>
-      <c r="F24" s="259"/>
-      <c r="G24" s="289"/>
+      <c r="F24" s="254"/>
+      <c r="G24" s="287"/>
       <c r="H24" s="238"/>
       <c r="I24" s="238"/>
-      <c r="J24" s="283"/>
+      <c r="J24" s="281"/>
       <c r="K24" s="238"/>
-      <c r="L24" s="210"/>
+      <c r="L24" s="212"/>
       <c r="M24" s="24"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -3706,18 +3863,18 @@
       <c r="AC24" s="4"/>
     </row>
     <row r="25" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A25" s="211"/>
-      <c r="B25" s="328"/>
-      <c r="C25" s="210"/>
-      <c r="D25" s="328"/>
+      <c r="A25" s="213"/>
+      <c r="B25" s="322"/>
+      <c r="C25" s="212"/>
+      <c r="D25" s="322"/>
       <c r="E25" s="247"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="290"/>
+      <c r="F25" s="255"/>
+      <c r="G25" s="288"/>
       <c r="H25" s="247"/>
       <c r="I25" s="238"/>
-      <c r="J25" s="284"/>
+      <c r="J25" s="282"/>
       <c r="K25" s="247"/>
-      <c r="L25" s="211"/>
+      <c r="L25" s="213"/>
       <c r="M25" s="24"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -3737,29 +3894,33 @@
       <c r="AC25" s="4"/>
     </row>
     <row r="26" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A26" s="299"/>
-      <c r="B26" s="212"/>
-      <c r="C26" s="212"/>
-      <c r="D26" s="328"/>
-      <c r="E26" s="296" t="s">
+      <c r="A26" s="294" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="214"/>
+      <c r="C26" s="214"/>
+      <c r="D26" s="322"/>
+      <c r="E26" s="289" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="289" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="296" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="285" t="s">
-        <v>117</v>
-      </c>
-      <c r="H26" s="285" t="s">
+      <c r="G26" s="283" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="283" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="238" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" s="308" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" s="217"/>
+      <c r="L26" s="211" t="s">
         <v>114</v>
-      </c>
-      <c r="I26" s="238" t="s">
-        <v>116</v>
-      </c>
-      <c r="J26" s="315"/>
-      <c r="K26" s="215"/>
-      <c r="L26" s="209" t="s">
-        <v>115</v>
       </c>
       <c r="M26" s="24"/>
       <c r="N26" s="4"/>
@@ -3780,18 +3941,18 @@
       <c r="AC26" s="4"/>
     </row>
     <row r="27" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A27" s="300"/>
-      <c r="B27" s="212"/>
-      <c r="C27" s="212"/>
-      <c r="D27" s="328"/>
-      <c r="E27" s="294"/>
-      <c r="F27" s="294"/>
-      <c r="G27" s="297"/>
-      <c r="H27" s="286"/>
+      <c r="A27" s="295"/>
+      <c r="B27" s="214"/>
+      <c r="C27" s="214"/>
+      <c r="D27" s="322"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="292"/>
+      <c r="H27" s="284"/>
       <c r="I27" s="238"/>
-      <c r="J27" s="283"/>
-      <c r="K27" s="216"/>
-      <c r="L27" s="210"/>
+      <c r="J27" s="281"/>
+      <c r="K27" s="218"/>
+      <c r="L27" s="212"/>
       <c r="M27" s="24"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -3811,18 +3972,18 @@
       <c r="AC27" s="4"/>
     </row>
     <row r="28" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A28" s="300"/>
-      <c r="B28" s="212"/>
-      <c r="C28" s="212"/>
-      <c r="D28" s="328"/>
-      <c r="E28" s="294"/>
-      <c r="F28" s="294"/>
-      <c r="G28" s="297"/>
-      <c r="H28" s="286"/>
+      <c r="A28" s="295"/>
+      <c r="B28" s="214"/>
+      <c r="C28" s="214"/>
+      <c r="D28" s="322"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="292"/>
+      <c r="H28" s="284"/>
       <c r="I28" s="238"/>
-      <c r="J28" s="283"/>
-      <c r="K28" s="216"/>
-      <c r="L28" s="210"/>
+      <c r="J28" s="281"/>
+      <c r="K28" s="218"/>
+      <c r="L28" s="212"/>
       <c r="M28" s="24"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -3842,18 +4003,18 @@
       <c r="AC28" s="4"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A29" s="300"/>
-      <c r="B29" s="212"/>
-      <c r="C29" s="212"/>
-      <c r="D29" s="328"/>
-      <c r="E29" s="294"/>
-      <c r="F29" s="294"/>
-      <c r="G29" s="297"/>
-      <c r="H29" s="286"/>
+      <c r="A29" s="295"/>
+      <c r="B29" s="214"/>
+      <c r="C29" s="214"/>
+      <c r="D29" s="322"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="292"/>
+      <c r="H29" s="284"/>
       <c r="I29" s="238"/>
-      <c r="J29" s="283"/>
-      <c r="K29" s="216"/>
-      <c r="L29" s="210"/>
+      <c r="J29" s="281"/>
+      <c r="K29" s="218"/>
+      <c r="L29" s="212"/>
       <c r="M29" s="24"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -3873,18 +4034,18 @@
       <c r="AC29" s="4"/>
     </row>
     <row r="30" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A30" s="300"/>
-      <c r="B30" s="212"/>
-      <c r="C30" s="212"/>
-      <c r="D30" s="328"/>
-      <c r="E30" s="294"/>
-      <c r="F30" s="294"/>
-      <c r="G30" s="297"/>
-      <c r="H30" s="286"/>
+      <c r="A30" s="295"/>
+      <c r="B30" s="214"/>
+      <c r="C30" s="214"/>
+      <c r="D30" s="322"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="292"/>
+      <c r="H30" s="284"/>
       <c r="I30" s="238"/>
-      <c r="J30" s="283"/>
-      <c r="K30" s="216"/>
-      <c r="L30" s="210"/>
+      <c r="J30" s="281"/>
+      <c r="K30" s="218"/>
+      <c r="L30" s="212"/>
       <c r="M30" s="24"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -3904,18 +4065,18 @@
       <c r="AC30" s="4"/>
     </row>
     <row r="31" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A31" s="300"/>
-      <c r="B31" s="212"/>
-      <c r="C31" s="212"/>
-      <c r="D31" s="328"/>
-      <c r="E31" s="294"/>
-      <c r="F31" s="294"/>
-      <c r="G31" s="297"/>
-      <c r="H31" s="286"/>
+      <c r="A31" s="295"/>
+      <c r="B31" s="214"/>
+      <c r="C31" s="214"/>
+      <c r="D31" s="322"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="292"/>
+      <c r="H31" s="284"/>
       <c r="I31" s="238"/>
-      <c r="J31" s="283"/>
-      <c r="K31" s="216"/>
-      <c r="L31" s="210"/>
+      <c r="J31" s="281"/>
+      <c r="K31" s="218"/>
+      <c r="L31" s="212"/>
       <c r="M31" s="24"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -3935,18 +4096,18 @@
       <c r="AC31" s="4"/>
     </row>
     <row r="32" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A32" s="301"/>
-      <c r="B32" s="212"/>
-      <c r="C32" s="212"/>
-      <c r="D32" s="328"/>
-      <c r="E32" s="295"/>
-      <c r="F32" s="295"/>
-      <c r="G32" s="298"/>
-      <c r="H32" s="287"/>
+      <c r="A32" s="296"/>
+      <c r="B32" s="214"/>
+      <c r="C32" s="214"/>
+      <c r="D32" s="322"/>
+      <c r="E32" s="291"/>
+      <c r="F32" s="291"/>
+      <c r="G32" s="293"/>
+      <c r="H32" s="285"/>
       <c r="I32" s="247"/>
-      <c r="J32" s="284"/>
-      <c r="K32" s="217"/>
-      <c r="L32" s="211"/>
+      <c r="J32" s="282"/>
+      <c r="K32" s="219"/>
+      <c r="L32" s="213"/>
       <c r="M32" s="24"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -3966,18 +4127,34 @@
       <c r="AC32" s="4"/>
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A33" s="299"/>
-      <c r="B33" s="212"/>
-      <c r="C33" s="212"/>
+      <c r="A33" s="294" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="214"/>
+      <c r="C33" s="214"/>
       <c r="D33" s="322"/>
-      <c r="E33" s="296"/>
-      <c r="F33" s="291"/>
-      <c r="G33" s="285"/>
-      <c r="H33" s="296"/>
-      <c r="I33" s="246"/>
-      <c r="J33" s="215"/>
-      <c r="K33" s="215"/>
-      <c r="L33" s="299"/>
+      <c r="E33" s="289" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="289" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="283" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" s="289" t="s">
+        <v>120</v>
+      </c>
+      <c r="I33" s="246" t="s">
+        <v>121</v>
+      </c>
+      <c r="J33" s="308" t="s">
+        <v>157</v>
+      </c>
+      <c r="K33" s="217"/>
+      <c r="L33" s="294" t="s">
+        <v>114</v>
+      </c>
       <c r="M33" s="24"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -3997,18 +4174,18 @@
       <c r="AC33" s="4"/>
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A34" s="300"/>
-      <c r="B34" s="212"/>
-      <c r="C34" s="212"/>
+      <c r="A34" s="295"/>
+      <c r="B34" s="214"/>
+      <c r="C34" s="214"/>
       <c r="D34" s="322"/>
-      <c r="E34" s="294"/>
-      <c r="F34" s="292"/>
-      <c r="G34" s="294"/>
-      <c r="H34" s="294"/>
+      <c r="E34" s="290"/>
+      <c r="F34" s="290"/>
+      <c r="G34" s="290"/>
+      <c r="H34" s="290"/>
       <c r="I34" s="238"/>
-      <c r="J34" s="216"/>
-      <c r="K34" s="216"/>
-      <c r="L34" s="300"/>
+      <c r="J34" s="281"/>
+      <c r="K34" s="218"/>
+      <c r="L34" s="295"/>
       <c r="M34" s="24"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -4028,18 +4205,18 @@
       <c r="AC34" s="4"/>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A35" s="300"/>
-      <c r="B35" s="212"/>
-      <c r="C35" s="212"/>
+      <c r="A35" s="295"/>
+      <c r="B35" s="214"/>
+      <c r="C35" s="214"/>
       <c r="D35" s="322"/>
-      <c r="E35" s="294"/>
-      <c r="F35" s="292"/>
-      <c r="G35" s="294"/>
-      <c r="H35" s="294"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
       <c r="I35" s="238"/>
-      <c r="J35" s="216"/>
-      <c r="K35" s="216"/>
-      <c r="L35" s="300"/>
+      <c r="J35" s="281"/>
+      <c r="K35" s="218"/>
+      <c r="L35" s="295"/>
       <c r="M35" s="20"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
@@ -4059,18 +4236,18 @@
       <c r="AC35" s="4"/>
     </row>
     <row r="36" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A36" s="300"/>
-      <c r="B36" s="212"/>
-      <c r="C36" s="212"/>
+      <c r="A36" s="295"/>
+      <c r="B36" s="214"/>
+      <c r="C36" s="214"/>
       <c r="D36" s="322"/>
-      <c r="E36" s="294"/>
-      <c r="F36" s="292"/>
-      <c r="G36" s="294"/>
-      <c r="H36" s="294"/>
+      <c r="E36" s="290"/>
+      <c r="F36" s="290"/>
+      <c r="G36" s="290"/>
+      <c r="H36" s="290"/>
       <c r="I36" s="238"/>
-      <c r="J36" s="216"/>
-      <c r="K36" s="216"/>
-      <c r="L36" s="300"/>
+      <c r="J36" s="281"/>
+      <c r="K36" s="218"/>
+      <c r="L36" s="295"/>
       <c r="M36" s="24"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -4090,18 +4267,18 @@
       <c r="AC36" s="4"/>
     </row>
     <row r="37" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A37" s="300"/>
-      <c r="B37" s="212"/>
-      <c r="C37" s="212"/>
+      <c r="A37" s="295"/>
+      <c r="B37" s="214"/>
+      <c r="C37" s="214"/>
       <c r="D37" s="322"/>
-      <c r="E37" s="294"/>
-      <c r="F37" s="292"/>
-      <c r="G37" s="294"/>
-      <c r="H37" s="294"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
       <c r="I37" s="238"/>
-      <c r="J37" s="216"/>
-      <c r="K37" s="216"/>
-      <c r="L37" s="300"/>
+      <c r="J37" s="281"/>
+      <c r="K37" s="218"/>
+      <c r="L37" s="295"/>
       <c r="M37" s="24"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
@@ -4121,18 +4298,18 @@
       <c r="AC37" s="4"/>
     </row>
     <row r="38" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A38" s="300"/>
-      <c r="B38" s="212"/>
-      <c r="C38" s="212"/>
+      <c r="A38" s="295"/>
+      <c r="B38" s="214"/>
+      <c r="C38" s="214"/>
       <c r="D38" s="322"/>
-      <c r="E38" s="294"/>
-      <c r="F38" s="292"/>
-      <c r="G38" s="294"/>
-      <c r="H38" s="294"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
       <c r="I38" s="238"/>
-      <c r="J38" s="216"/>
-      <c r="K38" s="216"/>
-      <c r="L38" s="300"/>
+      <c r="J38" s="281"/>
+      <c r="K38" s="218"/>
+      <c r="L38" s="295"/>
       <c r="M38" s="24"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -4152,18 +4329,18 @@
       <c r="AC38" s="4"/>
     </row>
     <row r="39" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A39" s="301"/>
-      <c r="B39" s="212"/>
-      <c r="C39" s="212"/>
+      <c r="A39" s="296"/>
+      <c r="B39" s="214"/>
+      <c r="C39" s="214"/>
       <c r="D39" s="322"/>
-      <c r="E39" s="295"/>
-      <c r="F39" s="293"/>
-      <c r="G39" s="295"/>
-      <c r="H39" s="295"/>
+      <c r="E39" s="291"/>
+      <c r="F39" s="291"/>
+      <c r="G39" s="291"/>
+      <c r="H39" s="291"/>
       <c r="I39" s="247"/>
-      <c r="J39" s="217"/>
-      <c r="K39" s="217"/>
-      <c r="L39" s="301"/>
+      <c r="J39" s="282"/>
+      <c r="K39" s="219"/>
+      <c r="L39" s="296"/>
       <c r="M39" s="24"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
@@ -4183,20 +4360,32 @@
       <c r="AC39" s="4"/>
     </row>
     <row r="40" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A40" s="316" t="s">
+      <c r="A40" s="309" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="212"/>
-      <c r="C40" s="212"/>
+      <c r="B40" s="214"/>
+      <c r="C40" s="214"/>
       <c r="D40" s="322"/>
-      <c r="E40" s="303"/>
-      <c r="F40" s="302"/>
-      <c r="G40" s="303"/>
-      <c r="H40" s="303"/>
-      <c r="I40" s="303"/>
-      <c r="J40" s="215"/>
-      <c r="K40" s="215"/>
-      <c r="L40" s="209"/>
+      <c r="E40" s="248" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="248" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="248" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" s="248" t="s">
+        <v>136</v>
+      </c>
+      <c r="I40" s="248" t="s">
+        <v>131</v>
+      </c>
+      <c r="J40" s="217"/>
+      <c r="K40" s="217"/>
+      <c r="L40" s="211" t="s">
+        <v>77</v>
+      </c>
       <c r="M40" s="27"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
@@ -4216,18 +4405,18 @@
       <c r="AC40" s="4"/>
     </row>
     <row r="41" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A41" s="300"/>
-      <c r="B41" s="212"/>
-      <c r="C41" s="212"/>
+      <c r="A41" s="295"/>
+      <c r="B41" s="214"/>
+      <c r="C41" s="214"/>
       <c r="D41" s="322"/>
       <c r="E41" s="238"/>
-      <c r="F41" s="216"/>
+      <c r="F41" s="238"/>
       <c r="G41" s="238"/>
       <c r="H41" s="238"/>
       <c r="I41" s="238"/>
-      <c r="J41" s="216"/>
-      <c r="K41" s="216"/>
-      <c r="L41" s="210"/>
+      <c r="J41" s="218"/>
+      <c r="K41" s="218"/>
+      <c r="L41" s="212"/>
       <c r="M41" s="28"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -4247,18 +4436,18 @@
       <c r="AC41" s="4"/>
     </row>
     <row r="42" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A42" s="300"/>
-      <c r="B42" s="212"/>
-      <c r="C42" s="212"/>
+      <c r="A42" s="295"/>
+      <c r="B42" s="214"/>
+      <c r="C42" s="214"/>
       <c r="D42" s="322"/>
       <c r="E42" s="238"/>
-      <c r="F42" s="216"/>
+      <c r="F42" s="238"/>
       <c r="G42" s="238"/>
       <c r="H42" s="238"/>
       <c r="I42" s="238"/>
-      <c r="J42" s="216"/>
-      <c r="K42" s="216"/>
-      <c r="L42" s="210"/>
+      <c r="J42" s="218"/>
+      <c r="K42" s="218"/>
+      <c r="L42" s="212"/>
       <c r="M42" s="28"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -4278,18 +4467,18 @@
       <c r="AC42" s="4"/>
     </row>
     <row r="43" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A43" s="300"/>
-      <c r="B43" s="212"/>
-      <c r="C43" s="212"/>
+      <c r="A43" s="295"/>
+      <c r="B43" s="214"/>
+      <c r="C43" s="214"/>
       <c r="D43" s="322"/>
       <c r="E43" s="238"/>
-      <c r="F43" s="216"/>
+      <c r="F43" s="238"/>
       <c r="G43" s="238"/>
       <c r="H43" s="238"/>
       <c r="I43" s="238"/>
-      <c r="J43" s="216"/>
-      <c r="K43" s="216"/>
-      <c r="L43" s="210"/>
+      <c r="J43" s="218"/>
+      <c r="K43" s="218"/>
+      <c r="L43" s="212"/>
       <c r="M43" s="28"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -4309,18 +4498,18 @@
       <c r="AC43" s="4"/>
     </row>
     <row r="44" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A44" s="300"/>
-      <c r="B44" s="212"/>
-      <c r="C44" s="212"/>
+      <c r="A44" s="295"/>
+      <c r="B44" s="214"/>
+      <c r="C44" s="214"/>
       <c r="D44" s="322"/>
       <c r="E44" s="238"/>
-      <c r="F44" s="216"/>
+      <c r="F44" s="238"/>
       <c r="G44" s="238"/>
       <c r="H44" s="238"/>
       <c r="I44" s="238"/>
-      <c r="J44" s="216"/>
-      <c r="K44" s="216"/>
-      <c r="L44" s="210"/>
+      <c r="J44" s="218"/>
+      <c r="K44" s="218"/>
+      <c r="L44" s="212"/>
       <c r="M44" s="28"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -4340,18 +4529,18 @@
       <c r="AC44" s="4"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A45" s="301"/>
-      <c r="B45" s="212"/>
-      <c r="C45" s="212"/>
+      <c r="A45" s="296"/>
+      <c r="B45" s="214"/>
+      <c r="C45" s="214"/>
       <c r="D45" s="322"/>
       <c r="E45" s="238"/>
-      <c r="F45" s="216"/>
+      <c r="F45" s="238"/>
       <c r="G45" s="247"/>
       <c r="H45" s="247"/>
       <c r="I45" s="247"/>
-      <c r="J45" s="217"/>
-      <c r="K45" s="217"/>
-      <c r="L45" s="211"/>
+      <c r="J45" s="219"/>
+      <c r="K45" s="219"/>
+      <c r="L45" s="213"/>
       <c r="M45" s="30"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
@@ -4371,20 +4560,34 @@
       <c r="AC45" s="4"/>
     </row>
     <row r="46" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A46" s="299" t="s">
+      <c r="A46" s="294" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="212"/>
-      <c r="C46" s="212"/>
-      <c r="D46" s="322"/>
-      <c r="E46" s="238"/>
-      <c r="F46" s="322"/>
-      <c r="G46" s="246"/>
-      <c r="H46" s="246"/>
-      <c r="I46" s="246"/>
-      <c r="J46" s="215"/>
-      <c r="K46" s="215"/>
-      <c r="L46" s="209"/>
+      <c r="B46" s="214"/>
+      <c r="C46" s="214"/>
+      <c r="D46" s="324" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="238" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="315" t="s">
+        <v>128</v>
+      </c>
+      <c r="G46" s="248" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="248" t="s">
+        <v>135</v>
+      </c>
+      <c r="I46" s="248" t="s">
+        <v>130</v>
+      </c>
+      <c r="J46" s="217"/>
+      <c r="K46" s="217"/>
+      <c r="L46" s="211" t="s">
+        <v>77</v>
+      </c>
       <c r="M46" s="30"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
@@ -4404,18 +4607,18 @@
       <c r="AC46" s="4"/>
     </row>
     <row r="47" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A47" s="300"/>
-      <c r="B47" s="212"/>
-      <c r="C47" s="212"/>
-      <c r="D47" s="322"/>
+      <c r="A47" s="295"/>
+      <c r="B47" s="214"/>
+      <c r="C47" s="214"/>
+      <c r="D47" s="324"/>
       <c r="E47" s="238"/>
-      <c r="F47" s="265"/>
+      <c r="F47" s="316"/>
       <c r="G47" s="238"/>
       <c r="H47" s="238"/>
       <c r="I47" s="238"/>
-      <c r="J47" s="216"/>
-      <c r="K47" s="216"/>
-      <c r="L47" s="210"/>
+      <c r="J47" s="218"/>
+      <c r="K47" s="218"/>
+      <c r="L47" s="212"/>
       <c r="M47" s="30"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -4435,18 +4638,18 @@
       <c r="AC47" s="4"/>
     </row>
     <row r="48" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A48" s="300"/>
-      <c r="B48" s="212"/>
-      <c r="C48" s="212"/>
-      <c r="D48" s="322"/>
+      <c r="A48" s="295"/>
+      <c r="B48" s="214"/>
+      <c r="C48" s="214"/>
+      <c r="D48" s="324"/>
       <c r="E48" s="238"/>
-      <c r="F48" s="265"/>
+      <c r="F48" s="316"/>
       <c r="G48" s="238"/>
       <c r="H48" s="238"/>
       <c r="I48" s="238"/>
-      <c r="J48" s="216"/>
-      <c r="K48" s="216"/>
-      <c r="L48" s="210"/>
+      <c r="J48" s="218"/>
+      <c r="K48" s="218"/>
+      <c r="L48" s="212"/>
       <c r="M48" s="30"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
@@ -4466,18 +4669,18 @@
       <c r="AC48" s="4"/>
     </row>
     <row r="49" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A49" s="300"/>
-      <c r="B49" s="212"/>
-      <c r="C49" s="212"/>
-      <c r="D49" s="322"/>
+      <c r="A49" s="295"/>
+      <c r="B49" s="214"/>
+      <c r="C49" s="214"/>
+      <c r="D49" s="324"/>
       <c r="E49" s="238"/>
-      <c r="F49" s="265"/>
+      <c r="F49" s="316"/>
       <c r="G49" s="238"/>
       <c r="H49" s="238"/>
       <c r="I49" s="238"/>
-      <c r="J49" s="216"/>
-      <c r="K49" s="216"/>
-      <c r="L49" s="210"/>
+      <c r="J49" s="218"/>
+      <c r="K49" s="218"/>
+      <c r="L49" s="212"/>
       <c r="M49" s="30"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
@@ -4497,18 +4700,18 @@
       <c r="AC49" s="4"/>
     </row>
     <row r="50" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A50" s="300"/>
-      <c r="B50" s="212"/>
-      <c r="C50" s="212"/>
-      <c r="D50" s="322"/>
+      <c r="A50" s="295"/>
+      <c r="B50" s="214"/>
+      <c r="C50" s="214"/>
+      <c r="D50" s="324"/>
       <c r="E50" s="238"/>
-      <c r="F50" s="265"/>
+      <c r="F50" s="316"/>
       <c r="G50" s="238"/>
       <c r="H50" s="238"/>
       <c r="I50" s="238"/>
-      <c r="J50" s="216"/>
-      <c r="K50" s="216"/>
-      <c r="L50" s="210"/>
+      <c r="J50" s="218"/>
+      <c r="K50" s="218"/>
+      <c r="L50" s="212"/>
       <c r="M50" s="30"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
@@ -4528,18 +4731,18 @@
       <c r="AC50" s="4"/>
     </row>
     <row r="51" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A51" s="301"/>
-      <c r="B51" s="212"/>
-      <c r="C51" s="212"/>
-      <c r="D51" s="323"/>
+      <c r="A51" s="296"/>
+      <c r="B51" s="214"/>
+      <c r="C51" s="214"/>
+      <c r="D51" s="324"/>
       <c r="E51" s="247"/>
-      <c r="F51" s="266"/>
+      <c r="F51" s="317"/>
       <c r="G51" s="247"/>
       <c r="H51" s="247"/>
       <c r="I51" s="247"/>
-      <c r="J51" s="217"/>
-      <c r="K51" s="217"/>
-      <c r="L51" s="211"/>
+      <c r="J51" s="219"/>
+      <c r="K51" s="219"/>
+      <c r="L51" s="213"/>
       <c r="M51" s="30"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
@@ -4559,20 +4762,32 @@
       <c r="AC51" s="4"/>
     </row>
     <row r="52" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A52" s="209" t="s">
+      <c r="A52" s="211" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="212"/>
-      <c r="C52" s="212"/>
-      <c r="D52" s="254"/>
-      <c r="E52" s="245"/>
-      <c r="F52" s="215"/>
-      <c r="G52" s="329"/>
-      <c r="H52" s="242"/>
-      <c r="I52" s="245"/>
-      <c r="J52" s="215"/>
-      <c r="K52" s="215"/>
-      <c r="L52" s="209"/>
+      <c r="B52" s="214"/>
+      <c r="C52" s="214"/>
+      <c r="D52" s="324"/>
+      <c r="E52" s="226" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="248" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" s="323" t="s">
+        <v>134</v>
+      </c>
+      <c r="H52" s="252" t="s">
+        <v>137</v>
+      </c>
+      <c r="I52" s="226" t="s">
+        <v>138</v>
+      </c>
+      <c r="J52" s="217"/>
+      <c r="K52" s="217"/>
+      <c r="L52" s="211" t="s">
+        <v>77</v>
+      </c>
       <c r="M52" s="30"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -4592,18 +4807,18 @@
       <c r="AC52" s="4"/>
     </row>
     <row r="53" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A53" s="210"/>
-      <c r="B53" s="212"/>
-      <c r="C53" s="212"/>
-      <c r="D53" s="255"/>
-      <c r="E53" s="213"/>
-      <c r="F53" s="216"/>
-      <c r="G53" s="259"/>
+      <c r="A53" s="212"/>
+      <c r="B53" s="214"/>
+      <c r="C53" s="214"/>
+      <c r="D53" s="324"/>
+      <c r="E53" s="215"/>
+      <c r="F53" s="238"/>
+      <c r="G53" s="254"/>
       <c r="H53" s="243"/>
-      <c r="I53" s="213"/>
-      <c r="J53" s="216"/>
-      <c r="K53" s="216"/>
-      <c r="L53" s="210"/>
+      <c r="I53" s="215"/>
+      <c r="J53" s="218"/>
+      <c r="K53" s="218"/>
+      <c r="L53" s="212"/>
       <c r="M53" s="17"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
@@ -4623,18 +4838,18 @@
       <c r="AC53" s="4"/>
     </row>
     <row r="54" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A54" s="210"/>
-      <c r="B54" s="212"/>
-      <c r="C54" s="212"/>
-      <c r="D54" s="255"/>
-      <c r="E54" s="213"/>
-      <c r="F54" s="216"/>
-      <c r="G54" s="259"/>
+      <c r="A54" s="212"/>
+      <c r="B54" s="214"/>
+      <c r="C54" s="214"/>
+      <c r="D54" s="324"/>
+      <c r="E54" s="215"/>
+      <c r="F54" s="238"/>
+      <c r="G54" s="254"/>
       <c r="H54" s="243"/>
-      <c r="I54" s="213"/>
-      <c r="J54" s="216"/>
-      <c r="K54" s="216"/>
-      <c r="L54" s="210"/>
+      <c r="I54" s="215"/>
+      <c r="J54" s="218"/>
+      <c r="K54" s="218"/>
+      <c r="L54" s="212"/>
       <c r="M54" s="24"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
@@ -4654,18 +4869,18 @@
       <c r="AC54" s="4"/>
     </row>
     <row r="55" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A55" s="210"/>
-      <c r="B55" s="212"/>
-      <c r="C55" s="212"/>
-      <c r="D55" s="255"/>
-      <c r="E55" s="213"/>
-      <c r="F55" s="216"/>
-      <c r="G55" s="259"/>
+      <c r="A55" s="212"/>
+      <c r="B55" s="214"/>
+      <c r="C55" s="214"/>
+      <c r="D55" s="324"/>
+      <c r="E55" s="215"/>
+      <c r="F55" s="238"/>
+      <c r="G55" s="254"/>
       <c r="H55" s="243"/>
-      <c r="I55" s="213"/>
-      <c r="J55" s="216"/>
-      <c r="K55" s="216"/>
-      <c r="L55" s="210"/>
+      <c r="I55" s="215"/>
+      <c r="J55" s="218"/>
+      <c r="K55" s="218"/>
+      <c r="L55" s="212"/>
       <c r="M55" s="24"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
@@ -4685,18 +4900,18 @@
       <c r="AC55" s="4"/>
     </row>
     <row r="56" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A56" s="210"/>
-      <c r="B56" s="212"/>
-      <c r="C56" s="212"/>
-      <c r="D56" s="255"/>
-      <c r="E56" s="213"/>
-      <c r="F56" s="216"/>
-      <c r="G56" s="259"/>
+      <c r="A56" s="212"/>
+      <c r="B56" s="214"/>
+      <c r="C56" s="214"/>
+      <c r="D56" s="324"/>
+      <c r="E56" s="215"/>
+      <c r="F56" s="238"/>
+      <c r="G56" s="254"/>
       <c r="H56" s="243"/>
-      <c r="I56" s="213"/>
-      <c r="J56" s="216"/>
-      <c r="K56" s="216"/>
-      <c r="L56" s="210"/>
+      <c r="I56" s="215"/>
+      <c r="J56" s="218"/>
+      <c r="K56" s="218"/>
+      <c r="L56" s="212"/>
       <c r="M56" s="24"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
@@ -4716,18 +4931,18 @@
       <c r="AC56" s="4"/>
     </row>
     <row r="57" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A57" s="211"/>
-      <c r="B57" s="212"/>
-      <c r="C57" s="212"/>
-      <c r="D57" s="255"/>
-      <c r="E57" s="214"/>
-      <c r="F57" s="217"/>
-      <c r="G57" s="259"/>
+      <c r="A57" s="213"/>
+      <c r="B57" s="214"/>
+      <c r="C57" s="214"/>
+      <c r="D57" s="324"/>
+      <c r="E57" s="216"/>
+      <c r="F57" s="247"/>
+      <c r="G57" s="254"/>
       <c r="H57" s="244"/>
-      <c r="I57" s="214"/>
-      <c r="J57" s="217"/>
-      <c r="K57" s="217"/>
-      <c r="L57" s="211"/>
+      <c r="I57" s="216"/>
+      <c r="J57" s="219"/>
+      <c r="K57" s="219"/>
+      <c r="L57" s="213"/>
       <c r="M57" s="27"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
@@ -4747,20 +4962,32 @@
       <c r="AC57" s="4"/>
     </row>
     <row r="58" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A58" s="209" t="s">
+      <c r="A58" s="211" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="212"/>
-      <c r="C58" s="212"/>
-      <c r="D58" s="255"/>
-      <c r="E58" s="245"/>
-      <c r="F58" s="215"/>
-      <c r="G58" s="259"/>
-      <c r="H58" s="256"/>
-      <c r="I58" s="251"/>
-      <c r="J58" s="215"/>
-      <c r="K58" s="228"/>
-      <c r="L58" s="209"/>
+      <c r="B58" s="214"/>
+      <c r="C58" s="214"/>
+      <c r="D58" s="324"/>
+      <c r="E58" s="226" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="248" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" s="253" t="s">
+        <v>152</v>
+      </c>
+      <c r="H58" s="256" t="s">
+        <v>141</v>
+      </c>
+      <c r="I58" s="226" t="s">
+        <v>142</v>
+      </c>
+      <c r="J58" s="217"/>
+      <c r="K58" s="230"/>
+      <c r="L58" s="211" t="s">
+        <v>77</v>
+      </c>
       <c r="M58" s="28"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
@@ -4780,18 +5007,18 @@
       <c r="AC58" s="4"/>
     </row>
     <row r="59" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A59" s="210"/>
-      <c r="B59" s="212"/>
-      <c r="C59" s="212"/>
-      <c r="D59" s="255"/>
-      <c r="E59" s="213"/>
-      <c r="F59" s="216"/>
-      <c r="G59" s="259"/>
+      <c r="A59" s="212"/>
+      <c r="B59" s="214"/>
+      <c r="C59" s="214"/>
+      <c r="D59" s="324"/>
+      <c r="E59" s="215"/>
+      <c r="F59" s="238"/>
+      <c r="G59" s="254"/>
       <c r="H59" s="257"/>
-      <c r="I59" s="252"/>
-      <c r="J59" s="216"/>
-      <c r="K59" s="229"/>
-      <c r="L59" s="210"/>
+      <c r="I59" s="215"/>
+      <c r="J59" s="218"/>
+      <c r="K59" s="231"/>
+      <c r="L59" s="212"/>
       <c r="M59" s="28"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -4811,18 +5038,18 @@
       <c r="AC59" s="4"/>
     </row>
     <row r="60" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A60" s="210"/>
-      <c r="B60" s="212"/>
-      <c r="C60" s="212"/>
-      <c r="D60" s="255"/>
-      <c r="E60" s="213"/>
-      <c r="F60" s="216"/>
-      <c r="G60" s="259"/>
+      <c r="A60" s="212"/>
+      <c r="B60" s="214"/>
+      <c r="C60" s="214"/>
+      <c r="D60" s="324"/>
+      <c r="E60" s="215"/>
+      <c r="F60" s="238"/>
+      <c r="G60" s="254"/>
       <c r="H60" s="257"/>
-      <c r="I60" s="252"/>
-      <c r="J60" s="216"/>
-      <c r="K60" s="229"/>
-      <c r="L60" s="210"/>
+      <c r="I60" s="215"/>
+      <c r="J60" s="218"/>
+      <c r="K60" s="231"/>
+      <c r="L60" s="212"/>
       <c r="M60" s="30"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
@@ -4842,18 +5069,18 @@
       <c r="AC60" s="4"/>
     </row>
     <row r="61" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A61" s="210"/>
-      <c r="B61" s="212"/>
-      <c r="C61" s="212"/>
-      <c r="D61" s="255"/>
-      <c r="E61" s="213"/>
-      <c r="F61" s="216"/>
-      <c r="G61" s="259"/>
+      <c r="A61" s="212"/>
+      <c r="B61" s="214"/>
+      <c r="C61" s="214"/>
+      <c r="D61" s="324"/>
+      <c r="E61" s="215"/>
+      <c r="F61" s="238"/>
+      <c r="G61" s="254"/>
       <c r="H61" s="257"/>
-      <c r="I61" s="252"/>
-      <c r="J61" s="216"/>
-      <c r="K61" s="229"/>
-      <c r="L61" s="210"/>
+      <c r="I61" s="215"/>
+      <c r="J61" s="218"/>
+      <c r="K61" s="231"/>
+      <c r="L61" s="212"/>
       <c r="M61" s="30"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -4873,18 +5100,18 @@
       <c r="AC61" s="4"/>
     </row>
     <row r="62" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A62" s="210"/>
-      <c r="B62" s="212"/>
-      <c r="C62" s="212"/>
-      <c r="D62" s="255"/>
-      <c r="E62" s="213"/>
-      <c r="F62" s="216"/>
-      <c r="G62" s="259"/>
+      <c r="A62" s="212"/>
+      <c r="B62" s="214"/>
+      <c r="C62" s="214"/>
+      <c r="D62" s="324"/>
+      <c r="E62" s="215"/>
+      <c r="F62" s="238"/>
+      <c r="G62" s="254"/>
       <c r="H62" s="257"/>
-      <c r="I62" s="252"/>
-      <c r="J62" s="216"/>
-      <c r="K62" s="229"/>
-      <c r="L62" s="210"/>
+      <c r="I62" s="215"/>
+      <c r="J62" s="218"/>
+      <c r="K62" s="231"/>
+      <c r="L62" s="212"/>
       <c r="M62" s="30"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -4904,18 +5131,18 @@
       <c r="AC62" s="4"/>
     </row>
     <row r="63" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A63" s="211"/>
-      <c r="B63" s="212"/>
-      <c r="C63" s="212"/>
-      <c r="D63" s="255"/>
-      <c r="E63" s="214"/>
-      <c r="F63" s="217"/>
-      <c r="G63" s="260"/>
+      <c r="A63" s="213"/>
+      <c r="B63" s="214"/>
+      <c r="C63" s="214"/>
+      <c r="D63" s="324"/>
+      <c r="E63" s="216"/>
+      <c r="F63" s="247"/>
+      <c r="G63" s="255"/>
       <c r="H63" s="258"/>
-      <c r="I63" s="253"/>
-      <c r="J63" s="217"/>
-      <c r="K63" s="230"/>
-      <c r="L63" s="211"/>
+      <c r="I63" s="216"/>
+      <c r="J63" s="219"/>
+      <c r="K63" s="232"/>
+      <c r="L63" s="213"/>
       <c r="M63" s="30"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
@@ -4935,20 +5162,34 @@
       <c r="AC63" s="4"/>
     </row>
     <row r="64" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A64" s="209" t="s">
+      <c r="A64" s="211" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="212"/>
-      <c r="C64" s="212"/>
-      <c r="D64" s="255"/>
-      <c r="E64" s="242"/>
-      <c r="F64" s="256"/>
-      <c r="G64" s="242"/>
-      <c r="H64" s="242"/>
-      <c r="I64" s="245"/>
-      <c r="J64" s="215"/>
-      <c r="K64" s="215"/>
-      <c r="L64" s="209"/>
+      <c r="B64" s="214"/>
+      <c r="C64" s="214"/>
+      <c r="D64" s="325" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="252" t="s">
+        <v>148</v>
+      </c>
+      <c r="F64" s="252" t="s">
+        <v>144</v>
+      </c>
+      <c r="G64" s="252" t="s">
+        <v>145</v>
+      </c>
+      <c r="H64" s="252" t="s">
+        <v>146</v>
+      </c>
+      <c r="I64" s="226" t="s">
+        <v>147</v>
+      </c>
+      <c r="J64" s="217"/>
+      <c r="K64" s="217"/>
+      <c r="L64" s="211" t="s">
+        <v>77</v>
+      </c>
       <c r="M64" s="30"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
@@ -4968,18 +5209,18 @@
       <c r="AC64" s="4"/>
     </row>
     <row r="65" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A65" s="210"/>
-      <c r="B65" s="212"/>
-      <c r="C65" s="212"/>
-      <c r="D65" s="255"/>
+      <c r="A65" s="212"/>
+      <c r="B65" s="214"/>
+      <c r="C65" s="214"/>
+      <c r="D65" s="324"/>
       <c r="E65" s="243"/>
-      <c r="F65" s="257"/>
+      <c r="F65" s="243"/>
       <c r="G65" s="243"/>
       <c r="H65" s="243"/>
-      <c r="I65" s="213"/>
-      <c r="J65" s="216"/>
-      <c r="K65" s="216"/>
-      <c r="L65" s="210"/>
+      <c r="I65" s="215"/>
+      <c r="J65" s="218"/>
+      <c r="K65" s="218"/>
+      <c r="L65" s="212"/>
       <c r="M65" s="24"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
@@ -4999,18 +5240,18 @@
       <c r="AC65" s="4"/>
     </row>
     <row r="66" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A66" s="210"/>
-      <c r="B66" s="212"/>
-      <c r="C66" s="212"/>
-      <c r="D66" s="255"/>
+      <c r="A66" s="212"/>
+      <c r="B66" s="214"/>
+      <c r="C66" s="214"/>
+      <c r="D66" s="324"/>
       <c r="E66" s="243"/>
-      <c r="F66" s="257"/>
+      <c r="F66" s="243"/>
       <c r="G66" s="243"/>
       <c r="H66" s="243"/>
-      <c r="I66" s="213"/>
-      <c r="J66" s="216"/>
-      <c r="K66" s="216"/>
-      <c r="L66" s="210"/>
+      <c r="I66" s="215"/>
+      <c r="J66" s="218"/>
+      <c r="K66" s="218"/>
+      <c r="L66" s="212"/>
       <c r="M66" s="24"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
@@ -5030,18 +5271,18 @@
       <c r="AC66" s="4"/>
     </row>
     <row r="67" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A67" s="210"/>
-      <c r="B67" s="212"/>
-      <c r="C67" s="212"/>
-      <c r="D67" s="255"/>
+      <c r="A67" s="212"/>
+      <c r="B67" s="214"/>
+      <c r="C67" s="214"/>
+      <c r="D67" s="324"/>
       <c r="E67" s="243"/>
-      <c r="F67" s="257"/>
+      <c r="F67" s="243"/>
       <c r="G67" s="243"/>
       <c r="H67" s="243"/>
-      <c r="I67" s="213"/>
-      <c r="J67" s="216"/>
-      <c r="K67" s="216"/>
-      <c r="L67" s="210"/>
+      <c r="I67" s="215"/>
+      <c r="J67" s="218"/>
+      <c r="K67" s="218"/>
+      <c r="L67" s="212"/>
       <c r="M67" s="24"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
@@ -5061,18 +5302,18 @@
       <c r="AC67" s="4"/>
     </row>
     <row r="68" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A68" s="210"/>
-      <c r="B68" s="212"/>
-      <c r="C68" s="212"/>
-      <c r="D68" s="255"/>
+      <c r="A68" s="212"/>
+      <c r="B68" s="214"/>
+      <c r="C68" s="214"/>
+      <c r="D68" s="324"/>
       <c r="E68" s="243"/>
-      <c r="F68" s="257"/>
+      <c r="F68" s="243"/>
       <c r="G68" s="243"/>
       <c r="H68" s="243"/>
-      <c r="I68" s="213"/>
-      <c r="J68" s="216"/>
-      <c r="K68" s="216"/>
-      <c r="L68" s="210"/>
+      <c r="I68" s="215"/>
+      <c r="J68" s="218"/>
+      <c r="K68" s="218"/>
+      <c r="L68" s="212"/>
       <c r="M68" s="24"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
@@ -5092,18 +5333,18 @@
       <c r="AC68" s="4"/>
     </row>
     <row r="69" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A69" s="211"/>
-      <c r="B69" s="212"/>
-      <c r="C69" s="212"/>
-      <c r="D69" s="255"/>
+      <c r="A69" s="213"/>
+      <c r="B69" s="214"/>
+      <c r="C69" s="214"/>
+      <c r="D69" s="324"/>
       <c r="E69" s="244"/>
-      <c r="F69" s="258"/>
+      <c r="F69" s="244"/>
       <c r="G69" s="244"/>
       <c r="H69" s="244"/>
-      <c r="I69" s="214"/>
-      <c r="J69" s="217"/>
-      <c r="K69" s="217"/>
-      <c r="L69" s="211"/>
+      <c r="I69" s="216"/>
+      <c r="J69" s="219"/>
+      <c r="K69" s="219"/>
+      <c r="L69" s="213"/>
       <c r="M69" s="24"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
@@ -5123,20 +5364,32 @@
       <c r="AC69" s="4"/>
     </row>
     <row r="70" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A70" s="209" t="s">
+      <c r="A70" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="212"/>
-      <c r="C70" s="212"/>
-      <c r="D70" s="231"/>
-      <c r="E70" s="246"/>
-      <c r="F70" s="215"/>
-      <c r="G70" s="248"/>
-      <c r="H70" s="246"/>
-      <c r="I70" s="246"/>
-      <c r="J70" s="215"/>
-      <c r="K70" s="215"/>
-      <c r="L70" s="209"/>
+      <c r="B70" s="214"/>
+      <c r="C70" s="214"/>
+      <c r="D70" s="324"/>
+      <c r="E70" s="248" t="s">
+        <v>149</v>
+      </c>
+      <c r="F70" s="248" t="s">
+        <v>150</v>
+      </c>
+      <c r="G70" s="249" t="s">
+        <v>151</v>
+      </c>
+      <c r="H70" s="248" t="s">
+        <v>153</v>
+      </c>
+      <c r="I70" s="248" t="s">
+        <v>154</v>
+      </c>
+      <c r="J70" s="217"/>
+      <c r="K70" s="217"/>
+      <c r="L70" s="211" t="s">
+        <v>77</v>
+      </c>
       <c r="M70" s="27"/>
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
@@ -5156,18 +5409,18 @@
       <c r="AC70" s="4"/>
     </row>
     <row r="71" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A71" s="210"/>
-      <c r="B71" s="212"/>
-      <c r="C71" s="212"/>
-      <c r="D71" s="231"/>
+      <c r="A71" s="212"/>
+      <c r="B71" s="214"/>
+      <c r="C71" s="214"/>
+      <c r="D71" s="324"/>
       <c r="E71" s="238"/>
-      <c r="F71" s="216"/>
-      <c r="G71" s="249"/>
+      <c r="F71" s="238"/>
+      <c r="G71" s="250"/>
       <c r="H71" s="238"/>
       <c r="I71" s="238"/>
-      <c r="J71" s="216"/>
-      <c r="K71" s="216"/>
-      <c r="L71" s="210"/>
+      <c r="J71" s="218"/>
+      <c r="K71" s="218"/>
+      <c r="L71" s="212"/>
       <c r="M71" s="28"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
@@ -5187,18 +5440,18 @@
       <c r="AC71" s="4"/>
     </row>
     <row r="72" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A72" s="210"/>
-      <c r="B72" s="212"/>
-      <c r="C72" s="212"/>
-      <c r="D72" s="231"/>
+      <c r="A72" s="212"/>
+      <c r="B72" s="214"/>
+      <c r="C72" s="214"/>
+      <c r="D72" s="324"/>
       <c r="E72" s="238"/>
-      <c r="F72" s="216"/>
-      <c r="G72" s="249"/>
+      <c r="F72" s="238"/>
+      <c r="G72" s="250"/>
       <c r="H72" s="238"/>
       <c r="I72" s="238"/>
-      <c r="J72" s="216"/>
-      <c r="K72" s="216"/>
-      <c r="L72" s="210"/>
+      <c r="J72" s="218"/>
+      <c r="K72" s="218"/>
+      <c r="L72" s="212"/>
       <c r="M72" s="28"/>
       <c r="N72" s="4"/>
       <c r="O72" s="4"/>
@@ -5218,18 +5471,18 @@
       <c r="AC72" s="4"/>
     </row>
     <row r="73" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A73" s="210"/>
-      <c r="B73" s="212"/>
-      <c r="C73" s="212"/>
-      <c r="D73" s="231"/>
+      <c r="A73" s="212"/>
+      <c r="B73" s="214"/>
+      <c r="C73" s="214"/>
+      <c r="D73" s="324"/>
       <c r="E73" s="238"/>
-      <c r="F73" s="216"/>
-      <c r="G73" s="249"/>
+      <c r="F73" s="238"/>
+      <c r="G73" s="250"/>
       <c r="H73" s="238"/>
       <c r="I73" s="238"/>
-      <c r="J73" s="216"/>
-      <c r="K73" s="216"/>
-      <c r="L73" s="210"/>
+      <c r="J73" s="218"/>
+      <c r="K73" s="218"/>
+      <c r="L73" s="212"/>
       <c r="M73" s="30"/>
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
@@ -5249,18 +5502,18 @@
       <c r="AC73" s="4"/>
     </row>
     <row r="74" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A74" s="210"/>
-      <c r="B74" s="212"/>
-      <c r="C74" s="212"/>
-      <c r="D74" s="231"/>
+      <c r="A74" s="212"/>
+      <c r="B74" s="214"/>
+      <c r="C74" s="214"/>
+      <c r="D74" s="324"/>
       <c r="E74" s="238"/>
-      <c r="F74" s="216"/>
-      <c r="G74" s="249"/>
+      <c r="F74" s="238"/>
+      <c r="G74" s="250"/>
       <c r="H74" s="238"/>
       <c r="I74" s="238"/>
-      <c r="J74" s="216"/>
-      <c r="K74" s="216"/>
-      <c r="L74" s="210"/>
+      <c r="J74" s="218"/>
+      <c r="K74" s="218"/>
+      <c r="L74" s="212"/>
       <c r="M74" s="24"/>
       <c r="N74" s="4"/>
       <c r="O74" s="4"/>
@@ -5280,18 +5533,18 @@
       <c r="AC74" s="4"/>
     </row>
     <row r="75" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A75" s="210"/>
-      <c r="B75" s="212"/>
-      <c r="C75" s="212"/>
-      <c r="D75" s="231"/>
+      <c r="A75" s="212"/>
+      <c r="B75" s="214"/>
+      <c r="C75" s="214"/>
+      <c r="D75" s="324"/>
       <c r="E75" s="238"/>
-      <c r="F75" s="216"/>
-      <c r="G75" s="249"/>
+      <c r="F75" s="238"/>
+      <c r="G75" s="250"/>
       <c r="H75" s="238"/>
       <c r="I75" s="238"/>
-      <c r="J75" s="216"/>
-      <c r="K75" s="216"/>
-      <c r="L75" s="210"/>
+      <c r="J75" s="218"/>
+      <c r="K75" s="218"/>
+      <c r="L75" s="212"/>
       <c r="M75" s="24"/>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
@@ -5311,18 +5564,18 @@
       <c r="AC75" s="4"/>
     </row>
     <row r="76" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A76" s="211"/>
-      <c r="B76" s="212"/>
-      <c r="C76" s="212"/>
-      <c r="D76" s="231"/>
+      <c r="A76" s="213"/>
+      <c r="B76" s="214"/>
+      <c r="C76" s="214"/>
+      <c r="D76" s="324"/>
       <c r="E76" s="238"/>
-      <c r="F76" s="217"/>
-      <c r="G76" s="250"/>
+      <c r="F76" s="247"/>
+      <c r="G76" s="251"/>
       <c r="H76" s="247"/>
       <c r="I76" s="247"/>
-      <c r="J76" s="217"/>
-      <c r="K76" s="217"/>
-      <c r="L76" s="211"/>
+      <c r="J76" s="219"/>
+      <c r="K76" s="219"/>
+      <c r="L76" s="213"/>
       <c r="M76" s="27"/>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -5347,15 +5600,15 @@
       </c>
       <c r="B77" s="236"/>
       <c r="C77" s="237"/>
-      <c r="D77" s="231"/>
+      <c r="D77" s="209"/>
       <c r="E77" s="238"/>
       <c r="F77" s="239"/>
       <c r="G77" s="242"/>
       <c r="H77" s="245"/>
       <c r="I77" s="246"/>
-      <c r="J77" s="215"/>
-      <c r="K77" s="228"/>
-      <c r="L77" s="209"/>
+      <c r="J77" s="217"/>
+      <c r="K77" s="230"/>
+      <c r="L77" s="211"/>
       <c r="M77" s="28"/>
       <c r="N77" s="4"/>
       <c r="O77" s="4"/>
@@ -5378,15 +5631,15 @@
       <c r="A78" s="234"/>
       <c r="B78" s="236"/>
       <c r="C78" s="237"/>
-      <c r="D78" s="231"/>
+      <c r="D78" s="209"/>
       <c r="E78" s="238"/>
       <c r="F78" s="240"/>
       <c r="G78" s="243"/>
-      <c r="H78" s="213"/>
+      <c r="H78" s="215"/>
       <c r="I78" s="238"/>
-      <c r="J78" s="216"/>
-      <c r="K78" s="229"/>
-      <c r="L78" s="210"/>
+      <c r="J78" s="218"/>
+      <c r="K78" s="231"/>
+      <c r="L78" s="212"/>
       <c r="M78" s="28"/>
       <c r="N78" s="4"/>
       <c r="O78" s="4"/>
@@ -5409,15 +5662,15 @@
       <c r="A79" s="234"/>
       <c r="B79" s="236"/>
       <c r="C79" s="237"/>
-      <c r="D79" s="231"/>
+      <c r="D79" s="209"/>
       <c r="E79" s="238"/>
       <c r="F79" s="240"/>
       <c r="G79" s="243"/>
-      <c r="H79" s="213"/>
+      <c r="H79" s="215"/>
       <c r="I79" s="238"/>
-      <c r="J79" s="216"/>
-      <c r="K79" s="229"/>
-      <c r="L79" s="210"/>
+      <c r="J79" s="218"/>
+      <c r="K79" s="231"/>
+      <c r="L79" s="212"/>
       <c r="M79" s="30"/>
       <c r="N79" s="4"/>
       <c r="O79" s="4"/>
@@ -5440,15 +5693,15 @@
       <c r="A80" s="234"/>
       <c r="B80" s="236"/>
       <c r="C80" s="237"/>
-      <c r="D80" s="231"/>
+      <c r="D80" s="209"/>
       <c r="E80" s="238"/>
       <c r="F80" s="240"/>
       <c r="G80" s="243"/>
-      <c r="H80" s="213"/>
+      <c r="H80" s="215"/>
       <c r="I80" s="238"/>
-      <c r="J80" s="216"/>
-      <c r="K80" s="229"/>
-      <c r="L80" s="210"/>
+      <c r="J80" s="218"/>
+      <c r="K80" s="231"/>
+      <c r="L80" s="212"/>
       <c r="M80" s="24"/>
       <c r="N80" s="4"/>
       <c r="O80" s="4"/>
@@ -5471,15 +5724,15 @@
       <c r="A81" s="234"/>
       <c r="B81" s="236"/>
       <c r="C81" s="237"/>
-      <c r="D81" s="231"/>
+      <c r="D81" s="209"/>
       <c r="E81" s="238"/>
       <c r="F81" s="240"/>
       <c r="G81" s="243"/>
-      <c r="H81" s="213"/>
+      <c r="H81" s="215"/>
       <c r="I81" s="238"/>
-      <c r="J81" s="216"/>
-      <c r="K81" s="229"/>
-      <c r="L81" s="210"/>
+      <c r="J81" s="218"/>
+      <c r="K81" s="231"/>
+      <c r="L81" s="212"/>
       <c r="M81" s="24"/>
       <c r="N81" s="4"/>
       <c r="O81" s="4"/>
@@ -5502,15 +5755,15 @@
       <c r="A82" s="235"/>
       <c r="B82" s="236"/>
       <c r="C82" s="237"/>
-      <c r="D82" s="231"/>
+      <c r="D82" s="209"/>
       <c r="E82" s="238"/>
       <c r="F82" s="241"/>
       <c r="G82" s="244"/>
-      <c r="H82" s="214"/>
+      <c r="H82" s="216"/>
       <c r="I82" s="247"/>
-      <c r="J82" s="217"/>
-      <c r="K82" s="230"/>
-      <c r="L82" s="211"/>
+      <c r="J82" s="219"/>
+      <c r="K82" s="232"/>
+      <c r="L82" s="213"/>
       <c r="M82" s="24"/>
       <c r="N82" s="4"/>
       <c r="O82" s="4"/>
@@ -5530,20 +5783,20 @@
       <c r="AC82" s="4"/>
     </row>
     <row r="83" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A83" s="209" t="s">
+      <c r="A83" s="211" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="212"/>
-      <c r="C83" s="212"/>
-      <c r="D83" s="231"/>
-      <c r="E83" s="213"/>
-      <c r="F83" s="215"/>
-      <c r="G83" s="218"/>
-      <c r="H83" s="221"/>
-      <c r="I83" s="224"/>
-      <c r="J83" s="225"/>
-      <c r="K83" s="228"/>
-      <c r="L83" s="209"/>
+      <c r="B83" s="214"/>
+      <c r="C83" s="214"/>
+      <c r="D83" s="209"/>
+      <c r="E83" s="215"/>
+      <c r="F83" s="217"/>
+      <c r="G83" s="220"/>
+      <c r="H83" s="223"/>
+      <c r="I83" s="226"/>
+      <c r="J83" s="227"/>
+      <c r="K83" s="230"/>
+      <c r="L83" s="211"/>
       <c r="M83" s="24"/>
       <c r="N83" s="4"/>
       <c r="O83" s="4"/>
@@ -5563,18 +5816,18 @@
       <c r="AC83" s="4"/>
     </row>
     <row r="84" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A84" s="210"/>
-      <c r="B84" s="212"/>
-      <c r="C84" s="212"/>
-      <c r="D84" s="231"/>
-      <c r="E84" s="213"/>
-      <c r="F84" s="216"/>
-      <c r="G84" s="219"/>
-      <c r="H84" s="222"/>
-      <c r="I84" s="213"/>
-      <c r="J84" s="226"/>
-      <c r="K84" s="229"/>
-      <c r="L84" s="210"/>
+      <c r="A84" s="212"/>
+      <c r="B84" s="214"/>
+      <c r="C84" s="214"/>
+      <c r="D84" s="209"/>
+      <c r="E84" s="215"/>
+      <c r="F84" s="218"/>
+      <c r="G84" s="221"/>
+      <c r="H84" s="224"/>
+      <c r="I84" s="215"/>
+      <c r="J84" s="228"/>
+      <c r="K84" s="231"/>
+      <c r="L84" s="212"/>
       <c r="M84" s="24"/>
       <c r="N84" s="4"/>
       <c r="O84" s="4"/>
@@ -5594,18 +5847,18 @@
       <c r="AC84" s="4"/>
     </row>
     <row r="85" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A85" s="210"/>
-      <c r="B85" s="212"/>
-      <c r="C85" s="212"/>
-      <c r="D85" s="231"/>
-      <c r="E85" s="213"/>
-      <c r="F85" s="216"/>
-      <c r="G85" s="219"/>
-      <c r="H85" s="222"/>
-      <c r="I85" s="213"/>
-      <c r="J85" s="226"/>
-      <c r="K85" s="229"/>
-      <c r="L85" s="210"/>
+      <c r="A85" s="212"/>
+      <c r="B85" s="214"/>
+      <c r="C85" s="214"/>
+      <c r="D85" s="209"/>
+      <c r="E85" s="215"/>
+      <c r="F85" s="218"/>
+      <c r="G85" s="221"/>
+      <c r="H85" s="224"/>
+      <c r="I85" s="215"/>
+      <c r="J85" s="228"/>
+      <c r="K85" s="231"/>
+      <c r="L85" s="212"/>
       <c r="M85" s="27"/>
       <c r="N85" s="4"/>
       <c r="O85" s="4"/>
@@ -5625,18 +5878,18 @@
       <c r="AC85" s="4"/>
     </row>
     <row r="86" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A86" s="210"/>
-      <c r="B86" s="212"/>
-      <c r="C86" s="212"/>
-      <c r="D86" s="231"/>
-      <c r="E86" s="213"/>
-      <c r="F86" s="216"/>
-      <c r="G86" s="219"/>
-      <c r="H86" s="222"/>
-      <c r="I86" s="213"/>
-      <c r="J86" s="226"/>
-      <c r="K86" s="229"/>
-      <c r="L86" s="210"/>
+      <c r="A86" s="212"/>
+      <c r="B86" s="214"/>
+      <c r="C86" s="214"/>
+      <c r="D86" s="209"/>
+      <c r="E86" s="215"/>
+      <c r="F86" s="218"/>
+      <c r="G86" s="221"/>
+      <c r="H86" s="224"/>
+      <c r="I86" s="215"/>
+      <c r="J86" s="228"/>
+      <c r="K86" s="231"/>
+      <c r="L86" s="212"/>
       <c r="M86" s="27"/>
       <c r="N86" s="4"/>
       <c r="O86" s="4"/>
@@ -5656,18 +5909,18 @@
       <c r="AC86" s="4"/>
     </row>
     <row r="87" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A87" s="210"/>
-      <c r="B87" s="212"/>
-      <c r="C87" s="212"/>
-      <c r="D87" s="231"/>
-      <c r="E87" s="213"/>
-      <c r="F87" s="216"/>
-      <c r="G87" s="219"/>
-      <c r="H87" s="222"/>
-      <c r="I87" s="213"/>
-      <c r="J87" s="226"/>
-      <c r="K87" s="229"/>
-      <c r="L87" s="210"/>
+      <c r="A87" s="212"/>
+      <c r="B87" s="214"/>
+      <c r="C87" s="214"/>
+      <c r="D87" s="209"/>
+      <c r="E87" s="215"/>
+      <c r="F87" s="218"/>
+      <c r="G87" s="221"/>
+      <c r="H87" s="224"/>
+      <c r="I87" s="215"/>
+      <c r="J87" s="228"/>
+      <c r="K87" s="231"/>
+      <c r="L87" s="212"/>
       <c r="M87" s="27"/>
       <c r="N87" s="4"/>
       <c r="O87" s="4"/>
@@ -5687,18 +5940,18 @@
       <c r="AC87" s="4"/>
     </row>
     <row r="88" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A88" s="211"/>
-      <c r="B88" s="212"/>
-      <c r="C88" s="212"/>
-      <c r="D88" s="232"/>
-      <c r="E88" s="214"/>
-      <c r="F88" s="217"/>
-      <c r="G88" s="220"/>
-      <c r="H88" s="223"/>
-      <c r="I88" s="214"/>
-      <c r="J88" s="227"/>
-      <c r="K88" s="230"/>
-      <c r="L88" s="211"/>
+      <c r="A88" s="213"/>
+      <c r="B88" s="214"/>
+      <c r="C88" s="214"/>
+      <c r="D88" s="210"/>
+      <c r="E88" s="216"/>
+      <c r="F88" s="219"/>
+      <c r="G88" s="222"/>
+      <c r="H88" s="225"/>
+      <c r="I88" s="216"/>
+      <c r="J88" s="229"/>
+      <c r="K88" s="232"/>
+      <c r="L88" s="213"/>
       <c r="M88" s="27"/>
       <c r="N88" s="4"/>
       <c r="O88" s="4"/>
@@ -5723,7 +5976,7 @@
       </c>
       <c r="B89" s="159"/>
       <c r="C89" s="162"/>
-      <c r="D89" s="269"/>
+      <c r="D89" s="267"/>
       <c r="E89" s="42"/>
       <c r="F89" s="200"/>
       <c r="G89" s="43"/>
@@ -5756,7 +6009,7 @@
       </c>
       <c r="B90" s="159"/>
       <c r="C90" s="162"/>
-      <c r="D90" s="262"/>
+      <c r="D90" s="260"/>
       <c r="E90" s="22"/>
       <c r="F90" s="195"/>
       <c r="G90" s="16"/>
@@ -5819,7 +6072,7 @@
       </c>
       <c r="B92" s="159"/>
       <c r="C92" s="162"/>
-      <c r="D92" s="268"/>
+      <c r="D92" s="266"/>
       <c r="E92" s="16"/>
       <c r="F92" s="195"/>
       <c r="G92" s="16"/>
@@ -5852,7 +6105,7 @@
       </c>
       <c r="B93" s="159"/>
       <c r="C93" s="162"/>
-      <c r="D93" s="262"/>
+      <c r="D93" s="260"/>
       <c r="E93" s="42"/>
       <c r="F93" s="200"/>
       <c r="G93" s="29"/>
@@ -5885,7 +6138,7 @@
       </c>
       <c r="B94" s="159"/>
       <c r="C94" s="162"/>
-      <c r="D94" s="262"/>
+      <c r="D94" s="260"/>
       <c r="E94" s="16"/>
       <c r="F94" s="195"/>
       <c r="G94" s="16"/>
@@ -5918,7 +6171,7 @@
       </c>
       <c r="B95" s="159"/>
       <c r="C95" s="162"/>
-      <c r="D95" s="262"/>
+      <c r="D95" s="260"/>
       <c r="E95" s="42"/>
       <c r="F95" s="200"/>
       <c r="G95" s="43"/>
@@ -5951,7 +6204,7 @@
       </c>
       <c r="B96" s="159"/>
       <c r="C96" s="162"/>
-      <c r="D96" s="262"/>
+      <c r="D96" s="260"/>
       <c r="E96" s="33"/>
       <c r="F96" s="196"/>
       <c r="G96" s="53"/>
@@ -5984,7 +6237,7 @@
       </c>
       <c r="B97" s="159"/>
       <c r="C97" s="162"/>
-      <c r="D97" s="262"/>
+      <c r="D97" s="260"/>
       <c r="E97" s="42"/>
       <c r="F97" s="200"/>
       <c r="G97" s="42"/>
@@ -6017,7 +6270,7 @@
       </c>
       <c r="B98" s="159"/>
       <c r="C98" s="162"/>
-      <c r="D98" s="263"/>
+      <c r="D98" s="261"/>
       <c r="E98" s="33"/>
       <c r="F98" s="196"/>
       <c r="G98" s="55"/>
@@ -6081,7 +6334,7 @@
       </c>
       <c r="B100" s="159"/>
       <c r="C100" s="162"/>
-      <c r="D100" s="273"/>
+      <c r="D100" s="271"/>
       <c r="E100" s="45"/>
       <c r="F100" s="32"/>
       <c r="G100" s="32"/>
@@ -6114,7 +6367,7 @@
       </c>
       <c r="B101" s="159"/>
       <c r="C101" s="162"/>
-      <c r="D101" s="274"/>
+      <c r="D101" s="272"/>
       <c r="E101" s="45"/>
       <c r="F101" s="196"/>
       <c r="G101" s="34"/>
@@ -6147,7 +6400,7 @@
       </c>
       <c r="B102" s="159"/>
       <c r="C102" s="162"/>
-      <c r="D102" s="274"/>
+      <c r="D102" s="272"/>
       <c r="E102" s="61"/>
       <c r="F102" s="197"/>
       <c r="G102" s="50"/>
@@ -6180,7 +6433,7 @@
       </c>
       <c r="B103" s="159"/>
       <c r="C103" s="162"/>
-      <c r="D103" s="274"/>
+      <c r="D103" s="272"/>
       <c r="E103" s="61"/>
       <c r="F103" s="197"/>
       <c r="G103" s="35"/>
@@ -6213,7 +6466,7 @@
       </c>
       <c r="B104" s="159"/>
       <c r="C104" s="162"/>
-      <c r="D104" s="274"/>
+      <c r="D104" s="272"/>
       <c r="E104" s="61"/>
       <c r="F104" s="197"/>
       <c r="G104" s="35"/>
@@ -6246,7 +6499,7 @@
       </c>
       <c r="B105" s="159"/>
       <c r="C105" s="162"/>
-      <c r="D105" s="274"/>
+      <c r="D105" s="272"/>
       <c r="E105" s="61"/>
       <c r="F105" s="197"/>
       <c r="G105" s="35"/>
@@ -6279,7 +6532,7 @@
       </c>
       <c r="B106" s="159"/>
       <c r="C106" s="162"/>
-      <c r="D106" s="274"/>
+      <c r="D106" s="272"/>
       <c r="E106" s="61"/>
       <c r="F106" s="197"/>
       <c r="G106" s="35"/>
@@ -6312,7 +6565,7 @@
       </c>
       <c r="B107" s="159"/>
       <c r="C107" s="162"/>
-      <c r="D107" s="274"/>
+      <c r="D107" s="272"/>
       <c r="E107" s="61"/>
       <c r="F107" s="197"/>
       <c r="G107" s="35"/>
@@ -6345,7 +6598,7 @@
       </c>
       <c r="B108" s="159"/>
       <c r="C108" s="162"/>
-      <c r="D108" s="275"/>
+      <c r="D108" s="273"/>
       <c r="E108" s="61"/>
       <c r="F108" s="197"/>
       <c r="G108" s="35"/>
@@ -6473,7 +6726,7 @@
       </c>
       <c r="B112" s="159"/>
       <c r="C112" s="30"/>
-      <c r="D112" s="270"/>
+      <c r="D112" s="268"/>
       <c r="E112" s="64"/>
       <c r="F112" s="201"/>
       <c r="G112" s="64"/>
@@ -6506,7 +6759,7 @@
       </c>
       <c r="B113" s="159"/>
       <c r="C113" s="30"/>
-      <c r="D113" s="263"/>
+      <c r="D113" s="261"/>
       <c r="E113" s="64"/>
       <c r="F113" s="201"/>
       <c r="G113" s="64"/>
@@ -7498,7 +7751,7 @@
       <c r="A145" s="72"/>
       <c r="B145" s="159"/>
       <c r="C145" s="30"/>
-      <c r="D145" s="271"/>
+      <c r="D145" s="269"/>
       <c r="E145" s="63"/>
       <c r="F145" s="197"/>
       <c r="G145" s="35"/>
@@ -7507,7 +7760,7 @@
       <c r="J145" s="35"/>
       <c r="K145" s="20"/>
       <c r="L145" s="26"/>
-      <c r="M145" s="278"/>
+      <c r="M145" s="276"/>
       <c r="N145" s="4"/>
       <c r="O145" s="4"/>
       <c r="P145" s="4"/>
@@ -7529,7 +7782,7 @@
       <c r="A146" s="19"/>
       <c r="B146" s="159"/>
       <c r="C146" s="30"/>
-      <c r="D146" s="262"/>
+      <c r="D146" s="260"/>
       <c r="E146" s="63"/>
       <c r="F146" s="197"/>
       <c r="G146" s="35"/>
@@ -7538,7 +7791,7 @@
       <c r="J146" s="35"/>
       <c r="K146" s="20"/>
       <c r="L146" s="26"/>
-      <c r="M146" s="262"/>
+      <c r="M146" s="260"/>
       <c r="N146" s="4"/>
       <c r="O146" s="4"/>
       <c r="P146" s="4"/>
@@ -7560,7 +7813,7 @@
       <c r="A147" s="19"/>
       <c r="B147" s="159"/>
       <c r="C147" s="30"/>
-      <c r="D147" s="262"/>
+      <c r="D147" s="260"/>
       <c r="E147" s="79"/>
       <c r="F147" s="197"/>
       <c r="G147" s="35"/>
@@ -7569,7 +7822,7 @@
       <c r="J147" s="35"/>
       <c r="K147" s="20"/>
       <c r="L147" s="26"/>
-      <c r="M147" s="262"/>
+      <c r="M147" s="260"/>
       <c r="N147" s="4"/>
       <c r="O147" s="4"/>
       <c r="P147" s="4"/>
@@ -7591,7 +7844,7 @@
       <c r="A148" s="19"/>
       <c r="B148" s="159"/>
       <c r="C148" s="30"/>
-      <c r="D148" s="262"/>
+      <c r="D148" s="260"/>
       <c r="E148" s="80"/>
       <c r="F148" s="179"/>
       <c r="G148" s="47"/>
@@ -7600,7 +7853,7 @@
       <c r="J148" s="35"/>
       <c r="K148" s="20"/>
       <c r="L148" s="26"/>
-      <c r="M148" s="262"/>
+      <c r="M148" s="260"/>
       <c r="N148" s="4"/>
       <c r="O148" s="4"/>
       <c r="P148" s="4"/>
@@ -7622,7 +7875,7 @@
       <c r="A149" s="19"/>
       <c r="B149" s="159"/>
       <c r="C149" s="30"/>
-      <c r="D149" s="262"/>
+      <c r="D149" s="260"/>
       <c r="E149" s="80"/>
       <c r="F149" s="179"/>
       <c r="G149" s="47"/>
@@ -7631,7 +7884,7 @@
       <c r="J149" s="35"/>
       <c r="K149" s="20"/>
       <c r="L149" s="26"/>
-      <c r="M149" s="262"/>
+      <c r="M149" s="260"/>
       <c r="N149" s="4"/>
       <c r="O149" s="4"/>
       <c r="P149" s="4"/>
@@ -7653,7 +7906,7 @@
       <c r="A150" s="19"/>
       <c r="B150" s="159"/>
       <c r="C150" s="30"/>
-      <c r="D150" s="262"/>
+      <c r="D150" s="260"/>
       <c r="E150" s="80"/>
       <c r="F150" s="179"/>
       <c r="G150" s="47"/>
@@ -7662,7 +7915,7 @@
       <c r="J150" s="35"/>
       <c r="K150" s="20"/>
       <c r="L150" s="26"/>
-      <c r="M150" s="262"/>
+      <c r="M150" s="260"/>
       <c r="N150" s="4"/>
       <c r="O150" s="4"/>
       <c r="P150" s="4"/>
@@ -7684,7 +7937,7 @@
       <c r="A151" s="19"/>
       <c r="B151" s="159"/>
       <c r="C151" s="30"/>
-      <c r="D151" s="262"/>
+      <c r="D151" s="260"/>
       <c r="E151" s="80"/>
       <c r="F151" s="179"/>
       <c r="G151" s="47"/>
@@ -7693,7 +7946,7 @@
       <c r="J151" s="35"/>
       <c r="K151" s="20"/>
       <c r="L151" s="26"/>
-      <c r="M151" s="262"/>
+      <c r="M151" s="260"/>
       <c r="N151" s="4"/>
       <c r="O151" s="4"/>
       <c r="P151" s="4"/>
@@ -7715,7 +7968,7 @@
       <c r="A152" s="19"/>
       <c r="B152" s="159"/>
       <c r="C152" s="30"/>
-      <c r="D152" s="262"/>
+      <c r="D152" s="260"/>
       <c r="E152" s="63"/>
       <c r="F152" s="197"/>
       <c r="G152" s="35"/>
@@ -7724,7 +7977,7 @@
       <c r="J152" s="35"/>
       <c r="K152" s="20"/>
       <c r="L152" s="26"/>
-      <c r="M152" s="263"/>
+      <c r="M152" s="261"/>
       <c r="N152" s="4"/>
       <c r="O152" s="4"/>
       <c r="P152" s="4"/>
@@ -7746,7 +7999,7 @@
       <c r="A153" s="19"/>
       <c r="B153" s="159"/>
       <c r="C153" s="30"/>
-      <c r="D153" s="262"/>
+      <c r="D153" s="260"/>
       <c r="E153" s="63"/>
       <c r="F153" s="197"/>
       <c r="G153" s="35"/>
@@ -7777,7 +8030,7 @@
       <c r="A154" s="19"/>
       <c r="B154" s="159"/>
       <c r="C154" s="30"/>
-      <c r="D154" s="262"/>
+      <c r="D154" s="260"/>
       <c r="E154" s="63"/>
       <c r="F154" s="197"/>
       <c r="G154" s="35"/>
@@ -7808,7 +8061,7 @@
       <c r="A155" s="19"/>
       <c r="B155" s="160"/>
       <c r="C155" s="30"/>
-      <c r="D155" s="262"/>
+      <c r="D155" s="260"/>
       <c r="E155" s="63"/>
       <c r="F155" s="197"/>
       <c r="G155" s="35"/>
@@ -7872,7 +8125,7 @@
       <c r="C157" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D157" s="272"/>
+      <c r="D157" s="270"/>
       <c r="E157" s="47"/>
       <c r="F157" s="197"/>
       <c r="G157" s="35"/>
@@ -7903,7 +8156,7 @@
       <c r="A158" s="19"/>
       <c r="B158" s="13"/>
       <c r="C158" s="82"/>
-      <c r="D158" s="262"/>
+      <c r="D158" s="260"/>
       <c r="E158" s="47"/>
       <c r="F158" s="197"/>
       <c r="G158" s="35"/>
@@ -7934,7 +8187,7 @@
       <c r="A159" s="19"/>
       <c r="B159" s="13"/>
       <c r="C159" s="82"/>
-      <c r="D159" s="262"/>
+      <c r="D159" s="260"/>
       <c r="E159" s="47"/>
       <c r="F159" s="197"/>
       <c r="G159" s="35"/>
@@ -7965,7 +8218,7 @@
       <c r="A160" s="19"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
-      <c r="D160" s="262"/>
+      <c r="D160" s="260"/>
       <c r="E160" s="83"/>
       <c r="F160" s="197"/>
       <c r="G160" s="35"/>
@@ -7996,7 +8249,7 @@
       <c r="A161" s="19"/>
       <c r="B161" s="26"/>
       <c r="C161" s="13"/>
-      <c r="D161" s="262"/>
+      <c r="D161" s="260"/>
       <c r="E161" s="83"/>
       <c r="F161" s="197"/>
       <c r="G161" s="35"/>
@@ -8027,7 +8280,7 @@
       <c r="A162" s="19"/>
       <c r="B162" s="26"/>
       <c r="C162" s="13"/>
-      <c r="D162" s="262"/>
+      <c r="D162" s="260"/>
       <c r="E162" s="83"/>
       <c r="F162" s="197"/>
       <c r="G162" s="35"/>
@@ -8058,7 +8311,7 @@
       <c r="A163" s="19"/>
       <c r="B163" s="26"/>
       <c r="C163" s="13"/>
-      <c r="D163" s="262"/>
+      <c r="D163" s="260"/>
       <c r="E163" s="47"/>
       <c r="F163" s="197"/>
       <c r="G163" s="35"/>
@@ -8089,7 +8342,7 @@
       <c r="A164" s="19"/>
       <c r="B164" s="26"/>
       <c r="C164" s="13"/>
-      <c r="D164" s="262"/>
+      <c r="D164" s="260"/>
       <c r="E164" s="47"/>
       <c r="F164" s="197"/>
       <c r="G164" s="35"/>
@@ -8120,7 +8373,7 @@
       <c r="A165" s="19"/>
       <c r="B165" s="26"/>
       <c r="C165" s="26"/>
-      <c r="D165" s="263"/>
+      <c r="D165" s="261"/>
       <c r="E165" s="47"/>
       <c r="F165" s="197"/>
       <c r="G165" s="35"/>
@@ -9460,8 +9713,8 @@
       <c r="H208" s="16"/>
       <c r="I208" s="36"/>
       <c r="J208" s="36"/>
-      <c r="K208" s="270"/>
-      <c r="L208" s="264"/>
+      <c r="K208" s="268"/>
+      <c r="L208" s="262"/>
       <c r="M208" s="17"/>
       <c r="N208" s="4"/>
       <c r="O208" s="4"/>
@@ -9491,8 +9744,8 @@
       <c r="H209" s="16"/>
       <c r="I209" s="48"/>
       <c r="J209" s="48"/>
-      <c r="K209" s="262"/>
-      <c r="L209" s="262"/>
+      <c r="K209" s="260"/>
+      <c r="L209" s="260"/>
       <c r="M209" s="17"/>
       <c r="N209" s="4"/>
       <c r="O209" s="4"/>
@@ -9522,8 +9775,8 @@
       <c r="H210" s="16"/>
       <c r="I210" s="41"/>
       <c r="J210" s="41"/>
-      <c r="K210" s="263"/>
-      <c r="L210" s="263"/>
+      <c r="K210" s="261"/>
+      <c r="L210" s="261"/>
       <c r="M210" s="17"/>
       <c r="N210" s="4"/>
       <c r="O210" s="4"/>
@@ -9731,10 +9984,10 @@
     <row r="217" spans="1:29" ht="15.75" customHeight="1">
       <c r="A217" s="19"/>
       <c r="B217" s="20"/>
-      <c r="C217" s="264"/>
+      <c r="C217" s="262"/>
       <c r="D217" s="13"/>
       <c r="E217" s="16"/>
-      <c r="F217" s="268"/>
+      <c r="F217" s="266"/>
       <c r="G217" s="16"/>
       <c r="H217" s="16"/>
       <c r="I217" s="16"/>
@@ -9762,10 +10015,10 @@
     <row r="218" spans="1:29" ht="15.75" customHeight="1">
       <c r="A218" s="19"/>
       <c r="B218" s="20"/>
-      <c r="C218" s="262"/>
+      <c r="C218" s="260"/>
       <c r="D218" s="13"/>
       <c r="E218" s="16"/>
-      <c r="F218" s="265"/>
+      <c r="F218" s="263"/>
       <c r="G218" s="16"/>
       <c r="H218" s="16"/>
       <c r="I218" s="16"/>
@@ -9793,10 +10046,10 @@
     <row r="219" spans="1:29" ht="15.75" customHeight="1">
       <c r="A219" s="19"/>
       <c r="B219" s="20"/>
-      <c r="C219" s="262"/>
+      <c r="C219" s="260"/>
       <c r="D219" s="13"/>
       <c r="E219" s="16"/>
-      <c r="F219" s="266"/>
+      <c r="F219" s="264"/>
       <c r="G219" s="16"/>
       <c r="H219" s="16"/>
       <c r="I219" s="16"/>
@@ -9824,7 +10077,7 @@
     <row r="220" spans="1:29" ht="15.75" customHeight="1">
       <c r="A220" s="19"/>
       <c r="B220" s="20"/>
-      <c r="C220" s="262"/>
+      <c r="C220" s="260"/>
       <c r="D220" s="13"/>
       <c r="E220" s="16"/>
       <c r="F220" s="195"/>
@@ -9855,7 +10108,7 @@
     <row r="221" spans="1:29" ht="15.75" customHeight="1">
       <c r="A221" s="19"/>
       <c r="B221" s="20"/>
-      <c r="C221" s="262"/>
+      <c r="C221" s="260"/>
       <c r="D221" s="13"/>
       <c r="E221" s="16"/>
       <c r="F221" s="195"/>
@@ -9886,7 +10139,7 @@
     <row r="222" spans="1:29" ht="15.75" customHeight="1">
       <c r="A222" s="19"/>
       <c r="B222" s="20"/>
-      <c r="C222" s="262"/>
+      <c r="C222" s="260"/>
       <c r="D222" s="13"/>
       <c r="E222" s="16"/>
       <c r="F222" s="195"/>
@@ -9917,7 +10170,7 @@
     <row r="223" spans="1:29" ht="15.75" customHeight="1">
       <c r="A223" s="19"/>
       <c r="B223" s="20"/>
-      <c r="C223" s="263"/>
+      <c r="C223" s="261"/>
       <c r="D223" s="13"/>
       <c r="E223" s="16"/>
       <c r="F223" s="195"/>
@@ -9948,7 +10201,7 @@
     <row r="224" spans="1:29" ht="15.75" customHeight="1">
       <c r="A224" s="19"/>
       <c r="B224" s="20"/>
-      <c r="C224" s="267"/>
+      <c r="C224" s="265"/>
       <c r="D224" s="87"/>
       <c r="E224" s="22"/>
       <c r="F224" s="195"/>
@@ -9979,7 +10232,7 @@
     <row r="225" spans="1:29" ht="15.75" customHeight="1">
       <c r="A225" s="19"/>
       <c r="B225" s="20"/>
-      <c r="C225" s="263"/>
+      <c r="C225" s="261"/>
       <c r="D225" s="83"/>
       <c r="E225" s="38"/>
       <c r="F225" s="195"/>
@@ -10041,7 +10294,7 @@
     <row r="227" spans="1:29" ht="30" customHeight="1">
       <c r="A227" s="19"/>
       <c r="B227" s="20"/>
-      <c r="C227" s="267"/>
+      <c r="C227" s="265"/>
       <c r="D227" s="87"/>
       <c r="E227" s="22"/>
       <c r="F227" s="195"/>
@@ -10072,7 +10325,7 @@
     <row r="228" spans="1:29" ht="15.75" customHeight="1">
       <c r="A228" s="19"/>
       <c r="B228" s="20"/>
-      <c r="C228" s="262"/>
+      <c r="C228" s="260"/>
       <c r="D228" s="49"/>
       <c r="E228" s="37"/>
       <c r="F228" s="195"/>
@@ -10103,7 +10356,7 @@
     <row r="229" spans="1:29" ht="15.75" customHeight="1">
       <c r="A229" s="19"/>
       <c r="B229" s="20"/>
-      <c r="C229" s="262"/>
+      <c r="C229" s="260"/>
       <c r="D229" s="49"/>
       <c r="E229" s="37"/>
       <c r="F229" s="195"/>
@@ -10134,7 +10387,7 @@
     <row r="230" spans="1:29" ht="15.75" customHeight="1">
       <c r="A230" s="19"/>
       <c r="B230" s="20"/>
-      <c r="C230" s="262"/>
+      <c r="C230" s="260"/>
       <c r="D230" s="49"/>
       <c r="E230" s="37"/>
       <c r="F230" s="195"/>
@@ -10165,7 +10418,7 @@
     <row r="231" spans="1:29" ht="15.75" customHeight="1">
       <c r="A231" s="19"/>
       <c r="B231" s="20"/>
-      <c r="C231" s="263"/>
+      <c r="C231" s="261"/>
       <c r="D231" s="49"/>
       <c r="E231" s="111"/>
       <c r="F231" s="182"/>
@@ -10545,7 +10798,7 @@
       <c r="H243" s="102"/>
       <c r="I243" s="102"/>
       <c r="J243" s="102"/>
-      <c r="K243" s="279"/>
+      <c r="K243" s="277"/>
       <c r="L243" s="26"/>
       <c r="M243" s="67"/>
       <c r="N243" s="4"/>
@@ -10576,7 +10829,7 @@
       <c r="H244" s="102"/>
       <c r="I244" s="102"/>
       <c r="J244" s="102"/>
-      <c r="K244" s="263"/>
+      <c r="K244" s="261"/>
       <c r="L244" s="26"/>
       <c r="M244" s="67"/>
       <c r="N244" s="4"/>
@@ -10661,7 +10914,7 @@
     <row r="247" spans="1:29" ht="15.75" customHeight="1">
       <c r="A247" s="19"/>
       <c r="B247" s="20"/>
-      <c r="C247" s="267"/>
+      <c r="C247" s="265"/>
       <c r="D247" s="87"/>
       <c r="E247" s="22"/>
       <c r="F247" s="195"/>
@@ -10669,7 +10922,7 @@
       <c r="H247" s="102"/>
       <c r="I247" s="102"/>
       <c r="J247" s="102"/>
-      <c r="K247" s="270"/>
+      <c r="K247" s="268"/>
       <c r="L247" s="26"/>
       <c r="M247" s="67"/>
       <c r="N247" s="4"/>
@@ -10692,7 +10945,7 @@
     <row r="248" spans="1:29" ht="15.75" customHeight="1">
       <c r="A248" s="19"/>
       <c r="B248" s="20"/>
-      <c r="C248" s="263"/>
+      <c r="C248" s="261"/>
       <c r="D248" s="83"/>
       <c r="E248" s="38"/>
       <c r="F248" s="195"/>
@@ -10700,7 +10953,7 @@
       <c r="H248" s="102"/>
       <c r="I248" s="102"/>
       <c r="J248" s="102"/>
-      <c r="K248" s="263"/>
+      <c r="K248" s="261"/>
       <c r="L248" s="26"/>
       <c r="M248" s="67"/>
       <c r="N248" s="4"/>
@@ -10723,7 +10976,7 @@
     <row r="249" spans="1:29" ht="15.75" customHeight="1">
       <c r="A249" s="19"/>
       <c r="B249" s="20"/>
-      <c r="C249" s="264"/>
+      <c r="C249" s="262"/>
       <c r="D249" s="18"/>
       <c r="E249" s="87"/>
       <c r="F249" s="197"/>
@@ -10754,7 +11007,7 @@
     <row r="250" spans="1:29" ht="15.75" customHeight="1">
       <c r="A250" s="19"/>
       <c r="B250" s="20"/>
-      <c r="C250" s="263"/>
+      <c r="C250" s="261"/>
       <c r="D250" s="65"/>
       <c r="E250" s="83"/>
       <c r="F250" s="197"/>
@@ -10816,7 +11069,7 @@
     <row r="252" spans="1:29" ht="15.75" customHeight="1">
       <c r="A252" s="19"/>
       <c r="B252" s="20"/>
-      <c r="C252" s="267"/>
+      <c r="C252" s="265"/>
       <c r="D252" s="87"/>
       <c r="E252" s="87"/>
       <c r="F252" s="197"/>
@@ -10847,7 +11100,7 @@
     <row r="253" spans="1:29" ht="15.75" customHeight="1">
       <c r="A253" s="19"/>
       <c r="B253" s="20"/>
-      <c r="C253" s="262"/>
+      <c r="C253" s="260"/>
       <c r="D253" s="49"/>
       <c r="E253" s="49"/>
       <c r="F253" s="197"/>
@@ -10878,7 +11131,7 @@
     <row r="254" spans="1:29" ht="15.75" customHeight="1">
       <c r="A254" s="19"/>
       <c r="B254" s="20"/>
-      <c r="C254" s="263"/>
+      <c r="C254" s="261"/>
       <c r="D254" s="83"/>
       <c r="E254" s="83"/>
       <c r="F254" s="197"/>
@@ -11063,11 +11316,11 @@
     </row>
     <row r="260" spans="1:29" ht="15.75" customHeight="1">
       <c r="A260" s="24"/>
-      <c r="B260" s="261"/>
-      <c r="C260" s="264"/>
+      <c r="B260" s="259"/>
+      <c r="C260" s="262"/>
       <c r="D260" s="13"/>
       <c r="E260" s="13"/>
-      <c r="F260" s="261"/>
+      <c r="F260" s="259"/>
       <c r="G260" s="121"/>
       <c r="H260" s="121"/>
       <c r="I260" s="121"/>
@@ -11094,11 +11347,11 @@
     </row>
     <row r="261" spans="1:29" ht="15.75" customHeight="1">
       <c r="A261" s="24"/>
-      <c r="B261" s="262"/>
-      <c r="C261" s="262"/>
+      <c r="B261" s="260"/>
+      <c r="C261" s="260"/>
       <c r="D261" s="13"/>
       <c r="E261" s="13"/>
-      <c r="F261" s="265"/>
+      <c r="F261" s="263"/>
       <c r="G261" s="121"/>
       <c r="H261" s="121"/>
       <c r="I261" s="121"/>
@@ -11125,11 +11378,11 @@
     </row>
     <row r="262" spans="1:29" ht="15.75" customHeight="1">
       <c r="A262" s="24"/>
-      <c r="B262" s="262"/>
-      <c r="C262" s="262"/>
+      <c r="B262" s="260"/>
+      <c r="C262" s="260"/>
       <c r="D262" s="13"/>
       <c r="E262" s="13"/>
-      <c r="F262" s="265"/>
+      <c r="F262" s="263"/>
       <c r="G262" s="121"/>
       <c r="H262" s="121"/>
       <c r="I262" s="121"/>
@@ -11156,11 +11409,11 @@
     </row>
     <row r="263" spans="1:29" ht="15.75" customHeight="1">
       <c r="A263" s="24"/>
-      <c r="B263" s="262"/>
-      <c r="C263" s="262"/>
+      <c r="B263" s="260"/>
+      <c r="C263" s="260"/>
       <c r="D263" s="13"/>
       <c r="E263" s="13"/>
-      <c r="F263" s="265"/>
+      <c r="F263" s="263"/>
       <c r="G263" s="121"/>
       <c r="H263" s="121"/>
       <c r="I263" s="121"/>
@@ -11187,11 +11440,11 @@
     </row>
     <row r="264" spans="1:29" ht="15.75" customHeight="1">
       <c r="A264" s="24"/>
-      <c r="B264" s="262"/>
-      <c r="C264" s="262"/>
+      <c r="B264" s="260"/>
+      <c r="C264" s="260"/>
       <c r="D264" s="13"/>
       <c r="E264" s="13"/>
-      <c r="F264" s="265"/>
+      <c r="F264" s="263"/>
       <c r="G264" s="121"/>
       <c r="H264" s="121"/>
       <c r="I264" s="121"/>
@@ -11218,11 +11471,11 @@
     </row>
     <row r="265" spans="1:29" ht="15.75" customHeight="1">
       <c r="A265" s="24"/>
-      <c r="B265" s="262"/>
-      <c r="C265" s="262"/>
+      <c r="B265" s="260"/>
+      <c r="C265" s="260"/>
       <c r="D265" s="13"/>
       <c r="E265" s="13"/>
-      <c r="F265" s="265"/>
+      <c r="F265" s="263"/>
       <c r="G265" s="122"/>
       <c r="H265" s="122"/>
       <c r="I265" s="122"/>
@@ -11249,11 +11502,11 @@
     </row>
     <row r="266" spans="1:29" ht="15.75" customHeight="1">
       <c r="A266" s="24"/>
-      <c r="B266" s="262"/>
-      <c r="C266" s="262"/>
+      <c r="B266" s="260"/>
+      <c r="C266" s="260"/>
       <c r="D266" s="13"/>
       <c r="E266" s="13"/>
-      <c r="F266" s="265"/>
+      <c r="F266" s="263"/>
       <c r="G266" s="121"/>
       <c r="H266" s="121"/>
       <c r="I266" s="121"/>
@@ -11280,11 +11533,11 @@
     </row>
     <row r="267" spans="1:29" ht="15.75" customHeight="1">
       <c r="A267" s="24"/>
-      <c r="B267" s="262"/>
-      <c r="C267" s="262"/>
+      <c r="B267" s="260"/>
+      <c r="C267" s="260"/>
       <c r="D267" s="13"/>
       <c r="E267" s="13"/>
-      <c r="F267" s="266"/>
+      <c r="F267" s="264"/>
       <c r="G267" s="121"/>
       <c r="H267" s="121"/>
       <c r="I267" s="121"/>
@@ -11311,8 +11564,8 @@
     </row>
     <row r="268" spans="1:29" ht="15.75" customHeight="1">
       <c r="A268" s="24"/>
-      <c r="B268" s="262"/>
-      <c r="C268" s="262"/>
+      <c r="B268" s="260"/>
+      <c r="C268" s="260"/>
       <c r="D268" s="13"/>
       <c r="E268" s="26"/>
       <c r="F268" s="85"/>
@@ -11342,8 +11595,8 @@
     </row>
     <row r="269" spans="1:29" ht="15.75" customHeight="1">
       <c r="A269" s="24"/>
-      <c r="B269" s="262"/>
-      <c r="C269" s="262"/>
+      <c r="B269" s="260"/>
+      <c r="C269" s="260"/>
       <c r="D269" s="13"/>
       <c r="E269" s="26"/>
       <c r="F269" s="85"/>
@@ -11373,11 +11626,11 @@
     </row>
     <row r="270" spans="1:29" ht="15.75" customHeight="1">
       <c r="A270" s="24"/>
-      <c r="B270" s="262"/>
-      <c r="C270" s="262"/>
+      <c r="B270" s="260"/>
+      <c r="C270" s="260"/>
       <c r="D270" s="18"/>
       <c r="E270" s="18"/>
-      <c r="F270" s="261"/>
+      <c r="F270" s="259"/>
       <c r="G270" s="28"/>
       <c r="H270" s="28"/>
       <c r="I270" s="28"/>
@@ -11404,11 +11657,11 @@
     </row>
     <row r="271" spans="1:29" ht="15.75" customHeight="1">
       <c r="A271" s="24"/>
-      <c r="B271" s="262"/>
-      <c r="C271" s="262"/>
+      <c r="B271" s="260"/>
+      <c r="C271" s="260"/>
       <c r="D271" s="81"/>
       <c r="E271" s="81"/>
-      <c r="F271" s="265"/>
+      <c r="F271" s="263"/>
       <c r="G271" s="24"/>
       <c r="H271" s="24"/>
       <c r="I271" s="24"/>
@@ -11435,11 +11688,11 @@
     </row>
     <row r="272" spans="1:29" ht="15.75" customHeight="1">
       <c r="A272" s="24"/>
-      <c r="B272" s="262"/>
-      <c r="C272" s="262"/>
+      <c r="B272" s="260"/>
+      <c r="C272" s="260"/>
       <c r="D272" s="81"/>
       <c r="E272" s="81"/>
-      <c r="F272" s="265"/>
+      <c r="F272" s="263"/>
       <c r="G272" s="24"/>
       <c r="H272" s="24"/>
       <c r="I272" s="24"/>
@@ -11466,11 +11719,11 @@
     </row>
     <row r="273" spans="1:29" ht="15.75" customHeight="1">
       <c r="A273" s="24"/>
-      <c r="B273" s="262"/>
-      <c r="C273" s="263"/>
+      <c r="B273" s="260"/>
+      <c r="C273" s="261"/>
       <c r="D273" s="65"/>
       <c r="E273" s="65"/>
-      <c r="F273" s="266"/>
+      <c r="F273" s="264"/>
       <c r="G273" s="24"/>
       <c r="H273" s="24"/>
       <c r="I273" s="24"/>
@@ -11497,7 +11750,7 @@
     </row>
     <row r="274" spans="1:29" ht="15.75" customHeight="1">
       <c r="A274" s="24"/>
-      <c r="B274" s="262"/>
+      <c r="B274" s="260"/>
       <c r="C274" s="13"/>
       <c r="D274" s="81"/>
       <c r="E274" s="81"/>
@@ -11528,11 +11781,11 @@
     </row>
     <row r="275" spans="1:29" ht="15.75" customHeight="1">
       <c r="A275" s="24"/>
-      <c r="B275" s="262"/>
-      <c r="C275" s="264"/>
+      <c r="B275" s="260"/>
+      <c r="C275" s="262"/>
       <c r="D275" s="18"/>
       <c r="E275" s="72"/>
-      <c r="F275" s="261"/>
+      <c r="F275" s="259"/>
       <c r="G275" s="35"/>
       <c r="H275" s="35"/>
       <c r="I275" s="35"/>
@@ -11559,11 +11812,11 @@
     </row>
     <row r="276" spans="1:29" ht="15.75" customHeight="1">
       <c r="A276" s="24"/>
-      <c r="B276" s="262"/>
-      <c r="C276" s="262"/>
+      <c r="B276" s="260"/>
+      <c r="C276" s="260"/>
       <c r="D276" s="65"/>
       <c r="E276" s="86"/>
-      <c r="F276" s="266"/>
+      <c r="F276" s="264"/>
       <c r="G276" s="35"/>
       <c r="H276" s="35"/>
       <c r="I276" s="35"/>
@@ -11590,11 +11843,11 @@
     </row>
     <row r="277" spans="1:29" ht="15.75" customHeight="1">
       <c r="A277" s="24"/>
-      <c r="B277" s="262"/>
-      <c r="C277" s="262"/>
+      <c r="B277" s="260"/>
+      <c r="C277" s="260"/>
       <c r="D277" s="13"/>
       <c r="E277" s="19"/>
-      <c r="F277" s="261"/>
+      <c r="F277" s="259"/>
       <c r="G277" s="35"/>
       <c r="H277" s="35"/>
       <c r="I277" s="35"/>
@@ -11621,11 +11874,11 @@
     </row>
     <row r="278" spans="1:29" ht="15.75" customHeight="1">
       <c r="A278" s="24"/>
-      <c r="B278" s="262"/>
-      <c r="C278" s="263"/>
+      <c r="B278" s="260"/>
+      <c r="C278" s="261"/>
       <c r="D278" s="13"/>
       <c r="E278" s="19"/>
-      <c r="F278" s="266"/>
+      <c r="F278" s="264"/>
       <c r="G278" s="35"/>
       <c r="H278" s="35"/>
       <c r="I278" s="35"/>
@@ -11652,7 +11905,7 @@
     </row>
     <row r="279" spans="1:29" ht="15.75" customHeight="1">
       <c r="A279" s="24"/>
-      <c r="B279" s="262"/>
+      <c r="B279" s="260"/>
       <c r="C279" s="26"/>
       <c r="D279" s="26"/>
       <c r="E279" s="24"/>
@@ -11683,11 +11936,11 @@
     </row>
     <row r="280" spans="1:29" ht="15.75" customHeight="1">
       <c r="A280" s="24"/>
-      <c r="B280" s="262"/>
-      <c r="C280" s="264"/>
+      <c r="B280" s="260"/>
+      <c r="C280" s="262"/>
       <c r="D280" s="18"/>
       <c r="E280" s="18"/>
-      <c r="F280" s="261"/>
+      <c r="F280" s="259"/>
       <c r="G280" s="28"/>
       <c r="H280" s="28"/>
       <c r="I280" s="28"/>
@@ -11714,11 +11967,11 @@
     </row>
     <row r="281" spans="1:29" ht="15.75" customHeight="1">
       <c r="A281" s="24"/>
-      <c r="B281" s="262"/>
-      <c r="C281" s="262"/>
+      <c r="B281" s="260"/>
+      <c r="C281" s="260"/>
       <c r="D281" s="81"/>
       <c r="E281" s="81"/>
-      <c r="F281" s="265"/>
+      <c r="F281" s="263"/>
       <c r="G281" s="28"/>
       <c r="H281" s="28"/>
       <c r="I281" s="28"/>
@@ -11745,11 +11998,11 @@
     </row>
     <row r="282" spans="1:29" ht="15.75" customHeight="1">
       <c r="A282" s="24"/>
-      <c r="B282" s="262"/>
-      <c r="C282" s="262"/>
+      <c r="B282" s="260"/>
+      <c r="C282" s="260"/>
       <c r="D282" s="81"/>
       <c r="E282" s="81"/>
-      <c r="F282" s="265"/>
+      <c r="F282" s="263"/>
       <c r="G282" s="28"/>
       <c r="H282" s="28"/>
       <c r="I282" s="28"/>
@@ -11776,11 +12029,11 @@
     </row>
     <row r="283" spans="1:29" ht="15.75" customHeight="1">
       <c r="A283" s="24"/>
-      <c r="B283" s="262"/>
-      <c r="C283" s="262"/>
+      <c r="B283" s="260"/>
+      <c r="C283" s="260"/>
       <c r="D283" s="81"/>
       <c r="E283" s="81"/>
-      <c r="F283" s="265"/>
+      <c r="F283" s="263"/>
       <c r="G283" s="28"/>
       <c r="H283" s="28"/>
       <c r="I283" s="28"/>
@@ -11807,11 +12060,11 @@
     </row>
     <row r="284" spans="1:29" ht="15.75" customHeight="1">
       <c r="A284" s="24"/>
-      <c r="B284" s="262"/>
-      <c r="C284" s="262"/>
+      <c r="B284" s="260"/>
+      <c r="C284" s="260"/>
       <c r="D284" s="81"/>
       <c r="E284" s="81"/>
-      <c r="F284" s="265"/>
+      <c r="F284" s="263"/>
       <c r="G284" s="121"/>
       <c r="H284" s="121"/>
       <c r="I284" s="121"/>
@@ -11838,11 +12091,11 @@
     </row>
     <row r="285" spans="1:29" ht="15.75" customHeight="1">
       <c r="A285" s="24"/>
-      <c r="B285" s="262"/>
-      <c r="C285" s="262"/>
+      <c r="B285" s="260"/>
+      <c r="C285" s="260"/>
       <c r="D285" s="65"/>
       <c r="E285" s="65"/>
-      <c r="F285" s="266"/>
+      <c r="F285" s="264"/>
       <c r="G285" s="121"/>
       <c r="H285" s="121"/>
       <c r="I285" s="121"/>
@@ -11869,11 +12122,11 @@
     </row>
     <row r="286" spans="1:29" ht="15.75" customHeight="1">
       <c r="A286" s="24"/>
-      <c r="B286" s="262"/>
-      <c r="C286" s="262"/>
+      <c r="B286" s="260"/>
+      <c r="C286" s="260"/>
       <c r="D286" s="18"/>
       <c r="E286" s="18"/>
-      <c r="F286" s="261"/>
+      <c r="F286" s="259"/>
       <c r="G286" s="28"/>
       <c r="H286" s="28"/>
       <c r="I286" s="28"/>
@@ -11900,11 +12153,11 @@
     </row>
     <row r="287" spans="1:29" ht="15.75" customHeight="1">
       <c r="A287" s="24"/>
-      <c r="B287" s="262"/>
-      <c r="C287" s="262"/>
+      <c r="B287" s="260"/>
+      <c r="C287" s="260"/>
       <c r="D287" s="81"/>
       <c r="E287" s="81"/>
-      <c r="F287" s="265"/>
+      <c r="F287" s="263"/>
       <c r="G287" s="24"/>
       <c r="H287" s="24"/>
       <c r="I287" s="24"/>
@@ -11931,11 +12184,11 @@
     </row>
     <row r="288" spans="1:29" ht="15.75" customHeight="1">
       <c r="A288" s="24"/>
-      <c r="B288" s="262"/>
-      <c r="C288" s="262"/>
+      <c r="B288" s="260"/>
+      <c r="C288" s="260"/>
       <c r="D288" s="81"/>
       <c r="E288" s="81"/>
-      <c r="F288" s="265"/>
+      <c r="F288" s="263"/>
       <c r="G288" s="24"/>
       <c r="H288" s="24"/>
       <c r="I288" s="24"/>
@@ -11962,11 +12215,11 @@
     </row>
     <row r="289" spans="1:29" ht="15.75" customHeight="1">
       <c r="A289" s="24"/>
-      <c r="B289" s="263"/>
-      <c r="C289" s="263"/>
+      <c r="B289" s="261"/>
+      <c r="C289" s="261"/>
       <c r="D289" s="65"/>
       <c r="E289" s="65"/>
-      <c r="F289" s="266"/>
+      <c r="F289" s="264"/>
       <c r="G289" s="24"/>
       <c r="H289" s="24"/>
       <c r="I289" s="24"/>
@@ -14741,7 +14994,7 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="168">
+  <mergeCells count="167">
     <mergeCell ref="J52:J57"/>
     <mergeCell ref="K52:K57"/>
     <mergeCell ref="L52:L57"/>
@@ -14753,6 +15006,7 @@
     <mergeCell ref="G52:G57"/>
     <mergeCell ref="H52:H57"/>
     <mergeCell ref="I52:I57"/>
+    <mergeCell ref="D46:D63"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L12:L18"/>
@@ -14764,9 +15018,9 @@
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="E12:E18"/>
     <mergeCell ref="L26:L32"/>
-    <mergeCell ref="D19:D32"/>
     <mergeCell ref="E26:E32"/>
     <mergeCell ref="E20:E25"/>
+    <mergeCell ref="D19:D45"/>
     <mergeCell ref="L40:L45"/>
     <mergeCell ref="D12:D18"/>
     <mergeCell ref="A12:A18"/>
@@ -14782,7 +15036,6 @@
     <mergeCell ref="J46:J51"/>
     <mergeCell ref="K46:K51"/>
     <mergeCell ref="L46:L51"/>
-    <mergeCell ref="D33:D51"/>
     <mergeCell ref="B46:B51"/>
     <mergeCell ref="C46:C51"/>
     <mergeCell ref="E46:E51"/>
@@ -14853,7 +15106,6 @@
     <mergeCell ref="F280:F285"/>
     <mergeCell ref="F286:F289"/>
     <mergeCell ref="C252:C254"/>
-    <mergeCell ref="I70:I76"/>
     <mergeCell ref="I58:I63"/>
     <mergeCell ref="J58:J63"/>
     <mergeCell ref="K58:K63"/>
@@ -14861,7 +15113,6 @@
     <mergeCell ref="A64:A69"/>
     <mergeCell ref="B64:B69"/>
     <mergeCell ref="C64:C69"/>
-    <mergeCell ref="D52:D69"/>
     <mergeCell ref="E64:E69"/>
     <mergeCell ref="F64:F69"/>
     <mergeCell ref="G64:G69"/>
@@ -14877,9 +15128,9 @@
     <mergeCell ref="F58:F63"/>
     <mergeCell ref="G58:G63"/>
     <mergeCell ref="H58:H63"/>
+    <mergeCell ref="D64:D76"/>
     <mergeCell ref="K83:K88"/>
     <mergeCell ref="L83:L88"/>
-    <mergeCell ref="D70:D88"/>
     <mergeCell ref="J70:J76"/>
     <mergeCell ref="K70:K76"/>
     <mergeCell ref="L70:L76"/>
@@ -14901,6 +15152,7 @@
     <mergeCell ref="F70:F76"/>
     <mergeCell ref="G70:G76"/>
     <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
     <mergeCell ref="A83:A88"/>
     <mergeCell ref="B83:B88"/>
     <mergeCell ref="C83:C88"/>
@@ -14938,10 +15190,12 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1"/>
+    <hyperlink ref="J26:J32" r:id="rId2" display="Click here"/>
+    <hyperlink ref="J33:J39" r:id="rId3" display="Click here"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -14972,39 +15226,39 @@
     <row r="2" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="3" spans="1:26" ht="8.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="25.5" customHeight="1">
-      <c r="B4" s="356" t="s">
+      <c r="B4" s="352" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="357"/>
-      <c r="D4" s="357"/>
-      <c r="E4" s="357"/>
-      <c r="F4" s="357"/>
-      <c r="G4" s="358"/>
+      <c r="C4" s="353"/>
+      <c r="D4" s="353"/>
+      <c r="E4" s="353"/>
+      <c r="F4" s="353"/>
+      <c r="G4" s="354"/>
       <c r="K4" s="128"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="B5" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="343" t="s">
+      <c r="C5" s="339" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="344"/>
-      <c r="E5" s="344"/>
-      <c r="F5" s="344"/>
-      <c r="G5" s="345"/>
+      <c r="D5" s="340"/>
+      <c r="E5" s="340"/>
+      <c r="F5" s="340"/>
+      <c r="G5" s="341"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="B6" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="343" t="s">
+      <c r="C6" s="339" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="344"/>
-      <c r="E6" s="344"/>
-      <c r="F6" s="344"/>
-      <c r="G6" s="345"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="340"/>
+      <c r="F6" s="340"/>
+      <c r="G6" s="341"/>
       <c r="I6" s="131" t="s">
         <v>24</v>
       </c>
@@ -15019,16 +15273,16 @@
       <c r="B7" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="343" t="s">
+      <c r="C7" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
-      <c r="F7" s="344"/>
-      <c r="G7" s="345"/>
+      <c r="D7" s="340"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="340"/>
+      <c r="G7" s="341"/>
       <c r="I7" s="133">
         <f>C15</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J7" s="134" t="s">
         <v>1</v>
@@ -15040,16 +15294,16 @@
       <c r="B8" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="343" t="s">
+      <c r="C8" s="339" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="344"/>
-      <c r="E8" s="344"/>
-      <c r="F8" s="344"/>
-      <c r="G8" s="345"/>
+      <c r="D8" s="340"/>
+      <c r="E8" s="340"/>
+      <c r="F8" s="340"/>
+      <c r="G8" s="341"/>
       <c r="I8" s="133">
         <f>D15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="134" t="s">
         <v>2</v>
@@ -15061,13 +15315,13 @@
       <c r="B9" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="343" t="s">
+      <c r="C9" s="339" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="344"/>
-      <c r="E9" s="344"/>
-      <c r="F9" s="344"/>
-      <c r="G9" s="345"/>
+      <c r="D9" s="340"/>
+      <c r="E9" s="340"/>
+      <c r="F9" s="340"/>
+      <c r="G9" s="341"/>
       <c r="I9" s="133">
         <f>E15</f>
         <v>0</v>
@@ -15091,13 +15345,13 @@
       <c r="B10" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="343" t="s">
+      <c r="C10" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="344"/>
-      <c r="E10" s="344"/>
-      <c r="F10" s="344"/>
-      <c r="G10" s="345"/>
+      <c r="D10" s="340"/>
+      <c r="E10" s="340"/>
+      <c r="F10" s="340"/>
+      <c r="G10" s="341"/>
       <c r="I10" s="133">
         <f>F15</f>
         <v>0</v>
@@ -15116,22 +15370,22 @@
       <c r="P10" s="52"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="B11" s="346" t="s">
+      <c r="B11" s="342" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="347"/>
-      <c r="D11" s="347"/>
-      <c r="E11" s="347"/>
-      <c r="F11" s="347"/>
-      <c r="G11" s="348"/>
+      <c r="C11" s="343"/>
+      <c r="D11" s="343"/>
+      <c r="E11" s="343"/>
+      <c r="F11" s="343"/>
+      <c r="G11" s="344"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="B12" s="340"/>
-      <c r="C12" s="341"/>
-      <c r="D12" s="341"/>
-      <c r="E12" s="341"/>
-      <c r="F12" s="341"/>
-      <c r="G12" s="342"/>
+      <c r="B12" s="336"/>
+      <c r="C12" s="337"/>
+      <c r="D12" s="337"/>
+      <c r="E12" s="337"/>
+      <c r="F12" s="337"/>
+      <c r="G12" s="338"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="B13" s="139" t="s">
@@ -15165,11 +15419,11 @@
       <c r="B14" s="144"/>
       <c r="C14" s="145">
         <f>TestCase!M5</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D14" s="146">
         <f>TestCase!M6</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="147">
         <f>TestCase!M7</f>
@@ -15181,7 +15435,7 @@
       </c>
       <c r="G14" s="149">
         <f>TestCase!M10</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H14" s="143"/>
       <c r="I14" s="143"/>
@@ -15209,11 +15463,11 @@
       </c>
       <c r="C15" s="152">
         <f t="shared" ref="C15:G15" si="0">SUM(C14)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D15" s="153">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="152">
         <f t="shared" si="0"/>
@@ -15225,7 +15479,7 @@
       </c>
       <c r="G15" s="154">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="L15" s="128"/>
       <c r="M15" s="155"/>
@@ -15266,21 +15520,21 @@
       <c r="R17" s="142"/>
     </row>
     <row r="18" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B18" s="349" t="s">
+      <c r="B18" s="345" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="350"/>
-      <c r="D18" s="350"/>
-      <c r="E18" s="350"/>
-      <c r="F18" s="350"/>
-      <c r="G18" s="277"/>
+      <c r="C18" s="346"/>
+      <c r="D18" s="346"/>
+      <c r="E18" s="346"/>
+      <c r="F18" s="346"/>
+      <c r="G18" s="275"/>
     </row>
     <row r="19" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B19" s="351" t="s">
+      <c r="B19" s="347" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="350"/>
-      <c r="D19" s="277"/>
+      <c r="C19" s="346"/>
+      <c r="D19" s="275"/>
       <c r="E19" s="157"/>
       <c r="F19" s="157" t="s">
         <v>45</v>
@@ -15290,11 +15544,11 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B20" s="352" t="s">
+      <c r="B20" s="348" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="350"/>
-      <c r="D20" s="277"/>
+      <c r="C20" s="346"/>
+      <c r="D20" s="275"/>
       <c r="E20" s="158"/>
       <c r="F20" s="158" t="s">
         <v>48</v>
@@ -15304,11 +15558,11 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B21" s="352" t="s">
+      <c r="B21" s="348" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="350"/>
-      <c r="D21" s="277"/>
+      <c r="C21" s="346"/>
+      <c r="D21" s="275"/>
       <c r="E21" s="158"/>
       <c r="F21" s="158" t="s">
         <v>48</v>
@@ -15319,306 +15573,306 @@
     </row>
     <row r="22" spans="2:18" ht="15.75" customHeight="1"/>
     <row r="23" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B23" s="355"/>
-      <c r="C23" s="353" t="s">
+      <c r="B23" s="351"/>
+      <c r="C23" s="349" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="354" t="s">
+      <c r="D23" s="350" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="336"/>
-      <c r="F23" s="336"/>
-      <c r="G23" s="337"/>
+      <c r="E23" s="332"/>
+      <c r="F23" s="332"/>
+      <c r="G23" s="333"/>
     </row>
     <row r="24" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B24" s="331"/>
-      <c r="C24" s="331"/>
-      <c r="D24" s="338"/>
-      <c r="E24" s="274"/>
-      <c r="F24" s="274"/>
-      <c r="G24" s="339"/>
+      <c r="B24" s="327"/>
+      <c r="C24" s="327"/>
+      <c r="D24" s="334"/>
+      <c r="E24" s="272"/>
+      <c r="F24" s="272"/>
+      <c r="G24" s="335"/>
     </row>
     <row r="25" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B25" s="331"/>
-      <c r="C25" s="331"/>
-      <c r="D25" s="338"/>
-      <c r="E25" s="274"/>
-      <c r="F25" s="274"/>
-      <c r="G25" s="339"/>
+      <c r="B25" s="327"/>
+      <c r="C25" s="327"/>
+      <c r="D25" s="334"/>
+      <c r="E25" s="272"/>
+      <c r="F25" s="272"/>
+      <c r="G25" s="335"/>
     </row>
     <row r="26" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B26" s="332"/>
-      <c r="C26" s="332"/>
-      <c r="D26" s="340"/>
-      <c r="E26" s="341"/>
-      <c r="F26" s="341"/>
-      <c r="G26" s="342"/>
+      <c r="B26" s="328"/>
+      <c r="C26" s="328"/>
+      <c r="D26" s="336"/>
+      <c r="E26" s="337"/>
+      <c r="F26" s="337"/>
+      <c r="G26" s="338"/>
     </row>
     <row r="27" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B27" s="333" t="s">
+      <c r="B27" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="330" t="s">
+      <c r="C27" s="326" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="335" t="s">
+      <c r="D27" s="331" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="336"/>
-      <c r="F27" s="336"/>
-      <c r="G27" s="337"/>
+      <c r="E27" s="332"/>
+      <c r="F27" s="332"/>
+      <c r="G27" s="333"/>
     </row>
     <row r="28" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B28" s="331"/>
-      <c r="C28" s="331"/>
-      <c r="D28" s="338"/>
-      <c r="E28" s="274"/>
-      <c r="F28" s="274"/>
-      <c r="G28" s="339"/>
+      <c r="B28" s="327"/>
+      <c r="C28" s="327"/>
+      <c r="D28" s="334"/>
+      <c r="E28" s="272"/>
+      <c r="F28" s="272"/>
+      <c r="G28" s="335"/>
     </row>
     <row r="29" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B29" s="331"/>
-      <c r="C29" s="331"/>
-      <c r="D29" s="338"/>
-      <c r="E29" s="274"/>
-      <c r="F29" s="274"/>
-      <c r="G29" s="339"/>
+      <c r="B29" s="327"/>
+      <c r="C29" s="327"/>
+      <c r="D29" s="334"/>
+      <c r="E29" s="272"/>
+      <c r="F29" s="272"/>
+      <c r="G29" s="335"/>
     </row>
     <row r="30" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B30" s="332"/>
-      <c r="C30" s="332"/>
-      <c r="D30" s="340"/>
-      <c r="E30" s="341"/>
-      <c r="F30" s="341"/>
-      <c r="G30" s="342"/>
+      <c r="B30" s="328"/>
+      <c r="C30" s="328"/>
+      <c r="D30" s="336"/>
+      <c r="E30" s="337"/>
+      <c r="F30" s="337"/>
+      <c r="G30" s="338"/>
     </row>
     <row r="31" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B31" s="333" t="s">
+      <c r="B31" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="330" t="s">
+      <c r="C31" s="326" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="335" t="s">
+      <c r="D31" s="331" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="336"/>
-      <c r="F31" s="336"/>
-      <c r="G31" s="337"/>
+      <c r="E31" s="332"/>
+      <c r="F31" s="332"/>
+      <c r="G31" s="333"/>
     </row>
     <row r="32" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B32" s="331"/>
-      <c r="C32" s="331"/>
-      <c r="D32" s="338"/>
-      <c r="E32" s="274"/>
-      <c r="F32" s="274"/>
-      <c r="G32" s="339"/>
+      <c r="B32" s="327"/>
+      <c r="C32" s="327"/>
+      <c r="D32" s="334"/>
+      <c r="E32" s="272"/>
+      <c r="F32" s="272"/>
+      <c r="G32" s="335"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B33" s="331"/>
-      <c r="C33" s="331"/>
-      <c r="D33" s="338"/>
-      <c r="E33" s="274"/>
-      <c r="F33" s="274"/>
-      <c r="G33" s="339"/>
+      <c r="B33" s="327"/>
+      <c r="C33" s="327"/>
+      <c r="D33" s="334"/>
+      <c r="E33" s="272"/>
+      <c r="F33" s="272"/>
+      <c r="G33" s="335"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B34" s="332"/>
-      <c r="C34" s="332"/>
-      <c r="D34" s="340"/>
-      <c r="E34" s="341"/>
-      <c r="F34" s="341"/>
-      <c r="G34" s="342"/>
+      <c r="B34" s="328"/>
+      <c r="C34" s="328"/>
+      <c r="D34" s="336"/>
+      <c r="E34" s="337"/>
+      <c r="F34" s="337"/>
+      <c r="G34" s="338"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B35" s="333" t="s">
+      <c r="B35" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="330" t="s">
+      <c r="C35" s="326" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="335" t="s">
+      <c r="D35" s="331" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="336"/>
-      <c r="F35" s="336"/>
-      <c r="G35" s="337"/>
+      <c r="E35" s="332"/>
+      <c r="F35" s="332"/>
+      <c r="G35" s="333"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B36" s="331"/>
-      <c r="C36" s="331"/>
-      <c r="D36" s="338"/>
-      <c r="E36" s="274"/>
-      <c r="F36" s="274"/>
-      <c r="G36" s="339"/>
+      <c r="B36" s="327"/>
+      <c r="C36" s="327"/>
+      <c r="D36" s="334"/>
+      <c r="E36" s="272"/>
+      <c r="F36" s="272"/>
+      <c r="G36" s="335"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B37" s="331"/>
-      <c r="C37" s="331"/>
-      <c r="D37" s="338"/>
-      <c r="E37" s="274"/>
-      <c r="F37" s="274"/>
-      <c r="G37" s="339"/>
+      <c r="B37" s="327"/>
+      <c r="C37" s="327"/>
+      <c r="D37" s="334"/>
+      <c r="E37" s="272"/>
+      <c r="F37" s="272"/>
+      <c r="G37" s="335"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B38" s="332"/>
-      <c r="C38" s="332"/>
-      <c r="D38" s="340"/>
-      <c r="E38" s="341"/>
-      <c r="F38" s="341"/>
-      <c r="G38" s="342"/>
+      <c r="B38" s="328"/>
+      <c r="C38" s="328"/>
+      <c r="D38" s="336"/>
+      <c r="E38" s="337"/>
+      <c r="F38" s="337"/>
+      <c r="G38" s="338"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B39" s="333" t="s">
+      <c r="B39" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="330" t="s">
+      <c r="C39" s="326" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="335" t="s">
+      <c r="D39" s="331" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="336"/>
-      <c r="F39" s="336"/>
-      <c r="G39" s="337"/>
+      <c r="E39" s="332"/>
+      <c r="F39" s="332"/>
+      <c r="G39" s="333"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B40" s="331"/>
-      <c r="C40" s="331"/>
-      <c r="D40" s="338"/>
-      <c r="E40" s="274"/>
-      <c r="F40" s="274"/>
-      <c r="G40" s="339"/>
+      <c r="B40" s="327"/>
+      <c r="C40" s="327"/>
+      <c r="D40" s="334"/>
+      <c r="E40" s="272"/>
+      <c r="F40" s="272"/>
+      <c r="G40" s="335"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B41" s="331"/>
-      <c r="C41" s="331"/>
-      <c r="D41" s="338"/>
-      <c r="E41" s="274"/>
-      <c r="F41" s="274"/>
-      <c r="G41" s="339"/>
+      <c r="B41" s="327"/>
+      <c r="C41" s="327"/>
+      <c r="D41" s="334"/>
+      <c r="E41" s="272"/>
+      <c r="F41" s="272"/>
+      <c r="G41" s="335"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B42" s="332"/>
-      <c r="C42" s="332"/>
-      <c r="D42" s="340"/>
-      <c r="E42" s="341"/>
-      <c r="F42" s="341"/>
-      <c r="G42" s="342"/>
+      <c r="B42" s="328"/>
+      <c r="C42" s="328"/>
+      <c r="D42" s="336"/>
+      <c r="E42" s="337"/>
+      <c r="F42" s="337"/>
+      <c r="G42" s="338"/>
     </row>
     <row r="43" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B43" s="333" t="s">
+      <c r="B43" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="334" t="s">
+      <c r="C43" s="330" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="335" t="s">
+      <c r="D43" s="331" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="336"/>
-      <c r="F43" s="336"/>
-      <c r="G43" s="337"/>
+      <c r="E43" s="332"/>
+      <c r="F43" s="332"/>
+      <c r="G43" s="333"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B44" s="331"/>
-      <c r="C44" s="331"/>
-      <c r="D44" s="338"/>
-      <c r="E44" s="274"/>
-      <c r="F44" s="274"/>
-      <c r="G44" s="339"/>
+      <c r="B44" s="327"/>
+      <c r="C44" s="327"/>
+      <c r="D44" s="334"/>
+      <c r="E44" s="272"/>
+      <c r="F44" s="272"/>
+      <c r="G44" s="335"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B45" s="331"/>
-      <c r="C45" s="331"/>
-      <c r="D45" s="338"/>
-      <c r="E45" s="274"/>
-      <c r="F45" s="274"/>
-      <c r="G45" s="339"/>
+      <c r="B45" s="327"/>
+      <c r="C45" s="327"/>
+      <c r="D45" s="334"/>
+      <c r="E45" s="272"/>
+      <c r="F45" s="272"/>
+      <c r="G45" s="335"/>
     </row>
     <row r="46" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B46" s="332"/>
-      <c r="C46" s="332"/>
-      <c r="D46" s="340"/>
-      <c r="E46" s="341"/>
-      <c r="F46" s="341"/>
-      <c r="G46" s="342"/>
+      <c r="B46" s="328"/>
+      <c r="C46" s="328"/>
+      <c r="D46" s="336"/>
+      <c r="E46" s="337"/>
+      <c r="F46" s="337"/>
+      <c r="G46" s="338"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B47" s="333" t="s">
+      <c r="B47" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="334" t="s">
+      <c r="C47" s="330" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="335" t="s">
+      <c r="D47" s="331" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="336"/>
-      <c r="F47" s="336"/>
-      <c r="G47" s="337"/>
+      <c r="E47" s="332"/>
+      <c r="F47" s="332"/>
+      <c r="G47" s="333"/>
     </row>
     <row r="48" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B48" s="331"/>
-      <c r="C48" s="331"/>
-      <c r="D48" s="338"/>
-      <c r="E48" s="274"/>
-      <c r="F48" s="274"/>
-      <c r="G48" s="339"/>
+      <c r="B48" s="327"/>
+      <c r="C48" s="327"/>
+      <c r="D48" s="334"/>
+      <c r="E48" s="272"/>
+      <c r="F48" s="272"/>
+      <c r="G48" s="335"/>
     </row>
     <row r="49" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B49" s="331"/>
-      <c r="C49" s="331"/>
-      <c r="D49" s="338"/>
-      <c r="E49" s="274"/>
-      <c r="F49" s="274"/>
-      <c r="G49" s="339"/>
+      <c r="B49" s="327"/>
+      <c r="C49" s="327"/>
+      <c r="D49" s="334"/>
+      <c r="E49" s="272"/>
+      <c r="F49" s="272"/>
+      <c r="G49" s="335"/>
     </row>
     <row r="50" spans="2:7" ht="33.75" customHeight="1">
-      <c r="B50" s="332"/>
-      <c r="C50" s="332"/>
-      <c r="D50" s="340"/>
-      <c r="E50" s="341"/>
-      <c r="F50" s="341"/>
-      <c r="G50" s="342"/>
+      <c r="B50" s="328"/>
+      <c r="C50" s="328"/>
+      <c r="D50" s="336"/>
+      <c r="E50" s="337"/>
+      <c r="F50" s="337"/>
+      <c r="G50" s="338"/>
     </row>
     <row r="51" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B51" s="333" t="s">
+      <c r="B51" s="329" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="334" t="s">
+      <c r="C51" s="330" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="335" t="s">
+      <c r="D51" s="331" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="336"/>
-      <c r="F51" s="336"/>
-      <c r="G51" s="337"/>
+      <c r="E51" s="332"/>
+      <c r="F51" s="332"/>
+      <c r="G51" s="333"/>
     </row>
     <row r="52" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B52" s="331"/>
-      <c r="C52" s="331"/>
-      <c r="D52" s="338"/>
-      <c r="E52" s="274"/>
-      <c r="F52" s="274"/>
-      <c r="G52" s="339"/>
+      <c r="B52" s="327"/>
+      <c r="C52" s="327"/>
+      <c r="D52" s="334"/>
+      <c r="E52" s="272"/>
+      <c r="F52" s="272"/>
+      <c r="G52" s="335"/>
     </row>
     <row r="53" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B53" s="331"/>
-      <c r="C53" s="331"/>
-      <c r="D53" s="338"/>
-      <c r="E53" s="274"/>
-      <c r="F53" s="274"/>
-      <c r="G53" s="339"/>
+      <c r="B53" s="327"/>
+      <c r="C53" s="327"/>
+      <c r="D53" s="334"/>
+      <c r="E53" s="272"/>
+      <c r="F53" s="272"/>
+      <c r="G53" s="335"/>
     </row>
     <row r="54" spans="2:7" ht="39" customHeight="1">
-      <c r="B54" s="332"/>
-      <c r="C54" s="332"/>
-      <c r="D54" s="340"/>
-      <c r="E54" s="341"/>
-      <c r="F54" s="341"/>
-      <c r="G54" s="342"/>
+      <c r="B54" s="328"/>
+      <c r="C54" s="328"/>
+      <c r="D54" s="336"/>
+      <c r="E54" s="337"/>
+      <c r="F54" s="337"/>
+      <c r="G54" s="338"/>
     </row>
     <row r="55" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="56" spans="2:7" ht="15.75" customHeight="1"/>

</xml_diff>